<commit_message>
rester fra i fjor
</commit_message>
<xml_diff>
--- a/marka24merge.xlsx
+++ b/marka24merge.xlsx
@@ -11,6 +11,7 @@
     <sheet name="DistanserMerge" sheetId="6" r:id="rId2"/>
     <sheet name="Ruteanalyse" sheetId="3" r:id="rId3"/>
     <sheet name="Lars vs Kris" sheetId="7" r:id="rId4"/>
+    <sheet name="TilProgrammet" sheetId="8" r:id="rId5"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -1819,11 +1820,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2133574520"/>
-        <c:axId val="-2133571464"/>
+        <c:axId val="-2133552248"/>
+        <c:axId val="-2133549192"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2133574520"/>
+        <c:axId val="-2133552248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1833,12 +1834,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2133571464"/>
+        <c:crossAx val="-2133549192"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2133571464"/>
+        <c:axId val="-2133549192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1849,7 +1850,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2133574520"/>
+        <c:crossAx val="-2133552248"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2617,8 +2618,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BC80"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AL6" sqref="AL6"/>
+    <sheetView tabSelected="1" topLeftCell="Q1" workbookViewId="0">
+      <selection activeCell="AF11" sqref="AF11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2894,27 +2895,27 @@
       </c>
       <c r="AE2" s="65">
         <f>AC2/AC$66*AA$66</f>
-        <v>1.8459339273750253</v>
+        <v>1.8536951074865262</v>
       </c>
       <c r="AF2" s="47">
         <f>IF(AE2&gt;AA2,AE2/AA2,AA2/AE2)-1</f>
-        <v>0.12090090109926677</v>
+        <v>0.12561369913150533</v>
       </c>
       <c r="AG2" s="75">
         <f>AVERAGE(AE2,AA2)</f>
-        <v>1.7463822743384001</v>
+        <v>1.7502628643941507</v>
       </c>
       <c r="AH2" s="65">
-        <f>AD2/AD$66*AB$66</f>
-        <v>0.82146807029636904</v>
+        <f>AD2/AC$66*AA$66</f>
+        <v>0.81768859647248415</v>
       </c>
       <c r="AI2" s="47">
         <f>IF(AH2&gt;AB2,AH2/AB2,AB2/AH2)-1</f>
-        <v>9.1741302833860283E-2</v>
+        <v>9.678748752362476E-2</v>
       </c>
       <c r="AJ2" s="76">
         <f>AVERAGE(AB2,AH2)</f>
-        <v>0.85914934579907198</v>
+        <v>0.8572596088871296</v>
       </c>
       <c r="AL2" s="25" t="s">
         <v>47</v>
@@ -3041,27 +3042,27 @@
       </c>
       <c r="AE3" s="65">
         <f t="shared" ref="AE3:AE64" si="10">AC3/AC$66*AA$66</f>
-        <v>1.2123406511417165</v>
+        <v>1.2174379051714885</v>
       </c>
       <c r="AF3" s="47">
         <f t="shared" ref="AF3:AF64" si="11">IF(AE3&gt;AA3,AE3/AA3,AA3/AE3)-1</f>
-        <v>2.324474110070307E-2</v>
+        <v>2.7546946405051065E-2</v>
       </c>
       <c r="AG3" s="75">
         <f t="shared" ref="AG3:AG64" si="12">AVERAGE(AE3,AA3)</f>
-        <v>1.198570463311905</v>
+        <v>1.2011190903267912</v>
       </c>
       <c r="AH3" s="65">
-        <f t="shared" ref="AH3:AH64" si="13">AD3/AD$66*AB$66</f>
-        <v>1.2954676579860911</v>
+        <f t="shared" ref="AH3:AH64" si="13">AD3/AC$66*AA$66</f>
+        <v>1.2895073702036559</v>
       </c>
       <c r="AI3" s="47">
         <f t="shared" ref="AI3:AI64" si="14">IF(AH3&gt;AB3,AH3/AB3,AB3/AH3)-1</f>
-        <v>5.138900406678526E-2</v>
+        <v>4.6551692230480723E-2</v>
       </c>
       <c r="AJ3" s="76">
         <f t="shared" ref="AJ3:AJ64" si="15">AVERAGE(AB3,AH3)</f>
-        <v>1.2638082091583347</v>
+        <v>1.2608280652671171</v>
       </c>
       <c r="AL3" s="25" t="s">
         <v>48</v>
@@ -3189,27 +3190,27 @@
       </c>
       <c r="AE4" s="65">
         <f t="shared" si="10"/>
-        <v>2.617037310634962</v>
+        <v>2.6280405744165862</v>
       </c>
       <c r="AF4" s="47">
         <f t="shared" si="11"/>
-        <v>9.322104195322356E-2</v>
+        <v>9.7817460753731655E-2</v>
       </c>
       <c r="AG4" s="75">
         <f t="shared" si="12"/>
-        <v>2.5054574308276854</v>
+        <v>2.5109590627184972</v>
       </c>
       <c r="AH4" s="65">
         <f t="shared" si="13"/>
-        <v>0.74649087542074244</v>
+        <v>0.74305636247320472</v>
       </c>
       <c r="AI4" s="47">
         <f t="shared" si="14"/>
-        <v>0.12396633350943165</v>
+        <v>0.12916146690710018</v>
       </c>
       <c r="AJ4" s="76">
         <f t="shared" si="15"/>
-        <v>0.79276074383282014</v>
+        <v>0.79104348735905128</v>
       </c>
       <c r="AL4" s="25" t="s">
         <v>51</v>
@@ -3392,27 +3393,27 @@
       </c>
       <c r="AE6" s="65">
         <f t="shared" si="10"/>
-        <v>2.716653522167229</v>
+        <v>2.7280756196612965</v>
       </c>
       <c r="AF6" s="47">
         <f t="shared" si="11"/>
-        <v>0.26483868440984337</v>
+        <v>0.27015666502449021</v>
       </c>
       <c r="AG6" s="75">
         <f t="shared" si="12"/>
-        <v>2.4322398045618754</v>
+        <v>2.4379508533089091</v>
       </c>
       <c r="AH6" s="65">
         <f t="shared" si="13"/>
-        <v>0.64777190698425247</v>
+        <v>0.6447915879008681</v>
       </c>
       <c r="AI6" s="47">
         <f t="shared" si="14"/>
-        <v>0.10076320163449726</v>
+        <v>0.10585108683287392</v>
       </c>
       <c r="AJ6" s="76">
         <f t="shared" si="15"/>
-        <v>0.68040769262256107</v>
+        <v>0.67891753308086877</v>
       </c>
       <c r="AL6" s="78" t="s">
         <v>88</v>
@@ -3598,27 +3599,27 @@
       </c>
       <c r="AE8" s="65">
         <f t="shared" si="10"/>
-        <v>2.4165598685573983</v>
+        <v>2.4267202302648028</v>
       </c>
       <c r="AF8" s="47">
         <f t="shared" si="11"/>
-        <v>2.2851706231994617E-2</v>
+        <v>2.7152259031688608E-2</v>
       </c>
       <c r="AG8" s="75">
         <f t="shared" si="12"/>
-        <v>2.3895654783286666</v>
+        <v>2.3946456591823688</v>
       </c>
       <c r="AH8" s="65">
         <f t="shared" si="13"/>
-        <v>1.6573738057340914</v>
+        <v>1.6497484321600402</v>
       </c>
       <c r="AI8" s="47">
         <f t="shared" si="14"/>
-        <v>5.2413952856585011E-2</v>
+        <v>4.7571925356626465E-2</v>
       </c>
       <c r="AJ8" s="76">
         <f t="shared" si="15"/>
-        <v>1.6161022546093204</v>
+        <v>1.612289567822295</v>
       </c>
       <c r="AL8" s="38" t="s">
         <v>45</v>
@@ -3746,27 +3747,27 @@
       </c>
       <c r="AE9" s="65">
         <f t="shared" si="10"/>
-        <v>1.4834061928215878</v>
+        <v>1.4896431347133143</v>
       </c>
       <c r="AF9" s="47">
         <f t="shared" si="11"/>
-        <v>6.8853168013339738E-2</v>
+        <v>7.3347132735845699E-2</v>
       </c>
       <c r="AG9" s="75">
         <f t="shared" si="12"/>
-        <v>1.4356273122031142</v>
+        <v>1.4387457831489774</v>
       </c>
       <c r="AH9" s="65">
         <f t="shared" si="13"/>
-        <v>1.1369668237887454</v>
+        <v>1.1317357789015288</v>
       </c>
       <c r="AI9" s="47">
         <f t="shared" si="14"/>
-        <v>2.3946200642831705E-2</v>
+        <v>1.9235149778736638E-2</v>
       </c>
       <c r="AJ9" s="76">
         <f t="shared" si="15"/>
-        <v>1.1236721625704138</v>
+        <v>1.1210566401268056</v>
       </c>
       <c r="AL9" s="38" t="s">
         <v>86</v>
@@ -3975,27 +3976,27 @@
       </c>
       <c r="AE11" s="65">
         <f t="shared" si="10"/>
-        <v>1.0902075384749419</v>
+        <v>1.094791287080209</v>
       </c>
       <c r="AF11" s="47">
         <f t="shared" si="11"/>
-        <v>1.5396643047233649E-2</v>
+        <v>1.1145309481386922E-2</v>
       </c>
       <c r="AG11" s="75">
         <f t="shared" si="12"/>
-        <v>1.098600306633593</v>
+        <v>1.1008921809362264</v>
       </c>
       <c r="AH11" s="65">
         <f t="shared" si="13"/>
-        <v>1.8305633533811536</v>
+        <v>1.8221411559431309</v>
       </c>
       <c r="AI11" s="47">
         <f t="shared" si="14"/>
-        <v>8.1140982254995331E-2</v>
+        <v>7.6166785216651434E-2</v>
       </c>
       <c r="AJ11" s="76">
         <f t="shared" si="15"/>
-        <v>1.7618703193498564</v>
+        <v>1.757659220630845</v>
       </c>
       <c r="AT11" s="9"/>
       <c r="AZ11" s="1"/>
@@ -4116,27 +4117,27 @@
       </c>
       <c r="AE12" s="65">
         <f t="shared" si="10"/>
-        <v>1.4625503176997805</v>
+        <v>1.4686995716191462</v>
       </c>
       <c r="AF12" s="47">
         <f t="shared" si="11"/>
-        <v>4.6053015344331927E-2</v>
+        <v>5.0451117431230985E-2</v>
       </c>
       <c r="AG12" s="75">
         <f t="shared" si="12"/>
-        <v>1.4303555573793802</v>
+        <v>1.4334301843390631</v>
       </c>
       <c r="AH12" s="65">
         <f t="shared" si="13"/>
-        <v>1.6999745460818356</v>
+        <v>1.6921531717271765</v>
       </c>
       <c r="AI12" s="47">
         <f t="shared" si="14"/>
-        <v>7.4007975426632511E-2</v>
+        <v>6.9066596477716846E-2</v>
       </c>
       <c r="AJ12" s="76">
         <f t="shared" si="15"/>
-        <v>1.6414034379937656</v>
+        <v>1.6374927508164361</v>
       </c>
       <c r="AT12" s="9"/>
       <c r="AZ12" s="1"/>
@@ -4257,27 +4258,27 @@
       </c>
       <c r="AE13" s="65">
         <f t="shared" si="10"/>
-        <v>1.1653193549433298</v>
+        <v>1.1702189091836024</v>
       </c>
       <c r="AF13" s="47">
         <f t="shared" si="11"/>
-        <v>1.3855052900200837E-2</v>
+        <v>9.6101737716243196E-3</v>
       </c>
       <c r="AG13" s="75">
         <f t="shared" si="12"/>
-        <v>1.1733921355975137</v>
+        <v>1.17584191271765</v>
       </c>
       <c r="AH13" s="65">
         <f t="shared" si="13"/>
-        <v>1.9159827254500581</v>
+        <v>1.9071675239593393</v>
       </c>
       <c r="AI13" s="47">
         <f t="shared" si="14"/>
-        <v>7.214834569952E-2</v>
+        <v>6.721552267886266E-2</v>
       </c>
       <c r="AJ13" s="76">
         <f t="shared" si="15"/>
-        <v>1.8515163740423672</v>
+        <v>1.8471087732970077</v>
       </c>
       <c r="AT13" s="9"/>
       <c r="AZ13" s="1"/>
@@ -4398,27 +4399,27 @@
       </c>
       <c r="AE14" s="65">
         <f t="shared" si="10"/>
-        <v>1.1717284585229704</v>
+        <v>1.1766549596688158</v>
       </c>
       <c r="AF14" s="47">
         <f t="shared" si="11"/>
-        <v>9.6332202765326613E-2</v>
+        <v>9.1742002546673751E-2</v>
       </c>
       <c r="AG14" s="75">
         <f t="shared" si="12"/>
-        <v>1.2281660502491394</v>
+        <v>1.2306293008220623</v>
       </c>
       <c r="AH14" s="65">
         <f t="shared" si="13"/>
-        <v>1.5661198393657074</v>
+        <v>1.5589143140970085</v>
       </c>
       <c r="AI14" s="47">
         <f t="shared" si="14"/>
-        <v>1.6812905481414342E-2</v>
+        <v>2.1512760385389296E-2</v>
       </c>
       <c r="AJ14" s="76">
         <f t="shared" si="15"/>
-        <v>1.5792853517816192</v>
+        <v>1.5756825891472697</v>
       </c>
       <c r="AT14" s="9"/>
       <c r="AZ14" s="1"/>
@@ -4539,27 +4540,27 @@
       </c>
       <c r="AE15" s="65">
         <f t="shared" si="10"/>
-        <v>1.6165026957451862</v>
+        <v>1.6232992383442197</v>
       </c>
       <c r="AF15" s="47">
         <f t="shared" si="11"/>
-        <v>5.7583538063926021E-2</v>
+        <v>6.2030119926985927E-2</v>
       </c>
       <c r="AG15" s="75">
         <f t="shared" si="12"/>
-        <v>1.5724948508985812</v>
+        <v>1.5758931221980979</v>
       </c>
       <c r="AH15" s="65">
         <f t="shared" si="13"/>
-        <v>2.4995588112296989</v>
+        <v>2.4880586477542086</v>
       </c>
       <c r="AI15" s="47">
         <f t="shared" si="14"/>
-        <v>4.4275689959980102E-2</v>
+        <v>3.9471105609307333E-2</v>
       </c>
       <c r="AJ15" s="76">
         <f t="shared" si="15"/>
-        <v>2.446570078452158</v>
+        <v>2.4408199967144131</v>
       </c>
       <c r="AK15"/>
       <c r="AL15"/>
@@ -4694,27 +4695,27 @@
       </c>
       <c r="AE16" s="65">
         <f t="shared" si="10"/>
-        <v>1.2167594074289012</v>
+        <v>1.2218752400019814</v>
       </c>
       <c r="AF16" s="47">
         <f t="shared" si="11"/>
-        <v>0.14660209764633447</v>
+        <v>0.14180142392166539</v>
       </c>
       <c r="AG16" s="75">
         <f t="shared" si="12"/>
-        <v>1.305949148158895</v>
+        <v>1.3085070644454353</v>
       </c>
       <c r="AH16" s="65">
         <f t="shared" si="13"/>
-        <v>2.5748691235394214</v>
+        <v>2.563022466555132</v>
       </c>
       <c r="AI16" s="47">
         <f t="shared" si="14"/>
-        <v>1.1108564090233752E-2</v>
+        <v>1.5782052711171835E-2</v>
       </c>
       <c r="AJ16" s="76">
         <f t="shared" si="15"/>
-        <v>2.5891706728808224</v>
+        <v>2.5832473443886776</v>
       </c>
       <c r="AK16"/>
       <c r="AL16"/>
@@ -4832,27 +4833,27 @@
       </c>
       <c r="AE17" s="65">
         <f t="shared" si="10"/>
-        <v>1.2218086778171753</v>
+        <v>1.2269457399133354</v>
       </c>
       <c r="AF17" s="47">
         <f t="shared" si="11"/>
-        <v>8.0909767474287131E-2</v>
+        <v>7.6384138984592509E-2</v>
       </c>
       <c r="AG17" s="75">
         <f t="shared" si="12"/>
-        <v>1.2712368058273023</v>
+        <v>1.2738053368753823</v>
       </c>
       <c r="AH17" s="65">
         <f t="shared" si="13"/>
-        <v>2.3405480450787506</v>
+        <v>2.3297794706328454</v>
       </c>
       <c r="AI17" s="47">
         <f t="shared" si="14"/>
-        <v>5.2457770518788305E-2</v>
+        <v>5.7322381094966346E-2</v>
       </c>
       <c r="AJ17" s="76">
         <f t="shared" si="15"/>
-        <v>2.4019380111972204</v>
+        <v>2.396553723974268</v>
       </c>
       <c r="AK17"/>
       <c r="AL17"/>
@@ -4987,27 +4988,27 @@
       </c>
       <c r="AE18" s="65">
         <f t="shared" si="10"/>
-        <v>2.1056091697800632</v>
+        <v>2.1144621475431027</v>
       </c>
       <c r="AF18" s="47">
         <f t="shared" si="11"/>
-        <v>0.1009543315454029</v>
+        <v>9.6344779075230313E-2</v>
       </c>
       <c r="AG18" s="75">
         <f t="shared" si="12"/>
-        <v>2.2118943528955715</v>
+        <v>2.2163208417770912</v>
       </c>
       <c r="AH18" s="65">
         <f t="shared" si="13"/>
-        <v>1.4582703241163368</v>
+        <v>1.451561001237655</v>
       </c>
       <c r="AI18" s="47">
         <f t="shared" si="14"/>
-        <v>9.4317760272230045E-2</v>
+        <v>9.9375853717343254E-2</v>
       </c>
       <c r="AJ18" s="76">
         <f t="shared" si="15"/>
-        <v>1.5270407195373927</v>
+        <v>1.5236860580980518</v>
       </c>
       <c r="AT18" s="9"/>
       <c r="AW18" s="9"/>
@@ -5129,27 +5130,27 @@
       </c>
       <c r="AE19" s="65">
         <f t="shared" si="10"/>
-        <v>1.1412434885537643</v>
+        <v>1.1460418164540154</v>
       </c>
       <c r="AF19" s="47">
         <f t="shared" si="11"/>
-        <v>0.11803209200350362</v>
+        <v>0.11335103717337947</v>
       </c>
       <c r="AG19" s="75">
         <f t="shared" si="12"/>
-        <v>1.2085951667734531</v>
+        <v>1.2109943307235786</v>
       </c>
       <c r="AH19" s="65">
         <f t="shared" si="13"/>
-        <v>0.94956250166606637</v>
+        <v>0.94519368107649071</v>
       </c>
       <c r="AI19" s="47">
         <f t="shared" si="14"/>
-        <v>0.18124339958423397</v>
+        <v>0.18670327578603674</v>
       </c>
       <c r="AJ19" s="76">
         <f t="shared" si="15"/>
-        <v>1.0356134696259003</v>
+        <v>1.0334290593311124</v>
       </c>
       <c r="AT19" s="9"/>
       <c r="AZ19" s="1"/>
@@ -5270,27 +5271,27 @@
       </c>
       <c r="AE20" s="65">
         <f t="shared" si="10"/>
-        <v>1.4668417368299607</v>
+        <v>1.4730090339069439</v>
       </c>
       <c r="AF20" s="47">
         <f t="shared" si="11"/>
-        <v>0.27509825442817148</v>
+        <v>0.26975958402195999</v>
       </c>
       <c r="AG20" s="75">
         <f t="shared" si="12"/>
-        <v>1.6686045374921155</v>
+        <v>1.671688186030607</v>
       </c>
       <c r="AH20" s="65">
         <f t="shared" si="13"/>
-        <v>1.3839588696583398</v>
+        <v>1.3775914446660085</v>
       </c>
       <c r="AI20" s="47">
         <f t="shared" si="14"/>
-        <v>0.27571550817517143</v>
+        <v>0.28161204799567585</v>
       </c>
       <c r="AJ20" s="76">
         <f t="shared" si="15"/>
-        <v>1.5747483311790322</v>
+        <v>1.5715646186828667</v>
       </c>
       <c r="AT20" s="9"/>
       <c r="AZ20" s="1"/>
@@ -5411,27 +5412,27 @@
       </c>
       <c r="AE21" s="65">
         <f t="shared" si="10"/>
-        <v>2.4773986958740832</v>
+        <v>2.4878148528131452</v>
       </c>
       <c r="AF21" s="47">
         <f t="shared" si="11"/>
-        <v>8.9148794902589534E-2</v>
+        <v>9.3728092048660283E-2</v>
       </c>
       <c r="AG21" s="75">
         <f t="shared" si="12"/>
-        <v>2.3760089182495419</v>
+        <v>2.3812169967190728</v>
       </c>
       <c r="AH21" s="65">
         <f t="shared" si="13"/>
-        <v>2.0929132689782683</v>
+        <v>2.0832840317604284</v>
       </c>
       <c r="AI21" s="47">
         <f t="shared" si="14"/>
-        <v>0.12577188092395697</v>
+        <v>0.12059234259560436</v>
       </c>
       <c r="AJ21" s="76">
         <f t="shared" si="15"/>
-        <v>1.9760025329266344</v>
+        <v>1.9711879143177145</v>
       </c>
       <c r="AT21" s="9"/>
       <c r="AZ21" s="1"/>
@@ -5552,27 +5553,27 @@
       </c>
       <c r="AE22" s="65">
         <f t="shared" si="10"/>
-        <v>3.5631783080889736</v>
+        <v>3.578159596535087</v>
       </c>
       <c r="AF22" s="47">
         <f t="shared" si="11"/>
-        <v>5.2431193658457165E-2</v>
+        <v>4.8024801250149629E-2</v>
       </c>
       <c r="AG22" s="75">
         <f t="shared" si="12"/>
-        <v>3.6565891540444868</v>
+        <v>3.6640797982675437</v>
       </c>
       <c r="AH22" s="65">
         <f t="shared" si="13"/>
-        <v>0.95858623006638244</v>
+        <v>0.95417589240935641</v>
       </c>
       <c r="AI22" s="47">
         <f t="shared" si="14"/>
-        <v>2.249197873747466E-2</v>
+        <v>1.7787618569980124E-2</v>
       </c>
       <c r="AJ22" s="76">
         <f t="shared" si="15"/>
-        <v>0.94804311503319116</v>
+        <v>0.9458379462046782</v>
       </c>
       <c r="AT22" s="9"/>
       <c r="AW22" s="9"/>
@@ -5694,27 +5695,27 @@
       </c>
       <c r="AE23" s="65">
         <f t="shared" si="10"/>
-        <v>1.4643310962876759</v>
+        <v>1.4704878374432608</v>
       </c>
       <c r="AF23" s="47">
         <f t="shared" si="11"/>
-        <v>9.8070008119635066E-3</v>
+        <v>1.4052707494597083E-2</v>
       </c>
       <c r="AG23" s="75">
         <f t="shared" si="12"/>
-        <v>1.4572204819629933</v>
+        <v>1.4602988525407858</v>
       </c>
       <c r="AH23" s="65">
         <f t="shared" si="13"/>
-        <v>1.6530254517155905</v>
+        <v>1.6454200843849762</v>
       </c>
       <c r="AI23" s="47">
         <f t="shared" si="14"/>
-        <v>3.4079743384624051E-2</v>
+        <v>2.9322069333431955E-2</v>
       </c>
       <c r="AJ23" s="76">
         <f t="shared" si="15"/>
-        <v>1.6257864096769505</v>
+        <v>1.6219837260116434</v>
       </c>
       <c r="AT23" s="9"/>
       <c r="AZ23" s="1"/>
@@ -5835,27 +5836,27 @@
       </c>
       <c r="AE24" s="65">
         <f t="shared" si="10"/>
-        <v>1.482138209364686</v>
+        <v>1.4883698200536857</v>
       </c>
       <c r="AF24" s="47">
         <f t="shared" si="11"/>
-        <v>1.5781737564930065E-2</v>
+        <v>1.1528791658466986E-2</v>
       </c>
       <c r="AG24" s="75">
         <f t="shared" si="12"/>
-        <v>1.4938335674922603</v>
+        <v>1.4969493728367602</v>
       </c>
       <c r="AH24" s="65">
         <f t="shared" si="13"/>
-        <v>1.8435356088231203</v>
+        <v>1.835053727629085</v>
       </c>
       <c r="AI24" s="47">
         <f t="shared" si="14"/>
-        <v>3.6164591098764021E-3</v>
+        <v>1.0020602267388767E-3</v>
       </c>
       <c r="AJ24" s="76">
         <f t="shared" si="15"/>
-        <v>1.8402140854032956</v>
+        <v>1.8359731448062782</v>
       </c>
       <c r="AT24" s="9"/>
       <c r="AZ24" s="1"/>
@@ -5976,27 +5977,27 @@
       </c>
       <c r="AE25" s="65">
         <f t="shared" si="10"/>
-        <v>1.5844457009342896</v>
+        <v>1.591107460751084</v>
       </c>
       <c r="AF25" s="47">
         <f t="shared" si="11"/>
-        <v>4.346928261741656E-3</v>
+        <v>8.5696782145292527E-3</v>
       </c>
       <c r="AG25" s="75">
         <f t="shared" si="12"/>
-        <v>1.5810168699184439</v>
+        <v>1.5843477498268412</v>
       </c>
       <c r="AH25" s="65">
         <f t="shared" si="13"/>
-        <v>1.619635378782341</v>
+        <v>1.6121836350814112</v>
       </c>
       <c r="AI25" s="47">
         <f t="shared" si="14"/>
-        <v>1.4785714336332134E-2</v>
+        <v>1.0116809746038236E-2</v>
       </c>
       <c r="AJ25" s="76">
         <f t="shared" si="15"/>
-        <v>1.607836106432831</v>
+        <v>1.6041102345823661</v>
       </c>
       <c r="AT25" s="9"/>
       <c r="AZ25" s="1"/>
@@ -6117,27 +6118,27 @@
       </c>
       <c r="AE26" s="65">
         <f t="shared" si="10"/>
-        <v>2.3059042436014305</v>
+        <v>2.3155993566762061</v>
       </c>
       <c r="AF26" s="47">
         <f t="shared" si="11"/>
-        <v>3.9588423793646355E-2</v>
+        <v>3.5235802390963578E-2</v>
       </c>
       <c r="AG26" s="75">
         <f t="shared" si="12"/>
-        <v>2.3515478008130613</v>
+        <v>2.3563953573504488</v>
       </c>
       <c r="AH26" s="65">
         <f t="shared" si="13"/>
-        <v>1.9513886630670789</v>
+        <v>1.9424105632005468</v>
       </c>
       <c r="AI26" s="47">
         <f t="shared" si="14"/>
-        <v>1.4930920140302284E-2</v>
+        <v>1.962207623844292E-2</v>
       </c>
       <c r="AJ26" s="76">
         <f t="shared" si="15"/>
-        <v>1.9659566772125519</v>
+        <v>1.9614676272792857</v>
       </c>
       <c r="AT26" s="9"/>
       <c r="AZ26" s="1"/>
@@ -6258,27 +6259,27 @@
       </c>
       <c r="AE27" s="65">
         <f t="shared" si="10"/>
-        <v>1.726161935918658</v>
+        <v>1.7334195378769972</v>
       </c>
       <c r="AF27" s="47">
         <f t="shared" si="11"/>
-        <v>4.4319059708145314E-2</v>
+        <v>4.8709871424680529E-2</v>
       </c>
       <c r="AG27" s="75">
         <f t="shared" si="12"/>
-        <v>1.6895343012926622</v>
+        <v>1.6931631022718319</v>
       </c>
       <c r="AH27" s="65">
         <f t="shared" si="13"/>
-        <v>1.0133625860701758</v>
+        <v>1.0087002291184624</v>
       </c>
       <c r="AI27" s="47">
         <f t="shared" si="14"/>
-        <v>9.8231454333165269E-2</v>
+        <v>0.10330763743285121</v>
       </c>
       <c r="AJ27" s="76">
         <f t="shared" si="15"/>
-        <v>1.0631346263684212</v>
+        <v>1.0608034478925643</v>
       </c>
       <c r="AT27" s="9"/>
       <c r="AW27" s="9"/>
@@ -6400,27 +6401,27 @@
       </c>
       <c r="AE28" s="65">
         <f t="shared" si="10"/>
-        <v>1.4759989057032668</v>
+        <v>1.4822047038532751</v>
       </c>
       <c r="AF28" s="47">
         <f t="shared" si="11"/>
-        <v>0.18683103466105511</v>
+        <v>0.19182103418667329</v>
       </c>
       <c r="AG28" s="75">
         <f t="shared" si="12"/>
-        <v>1.3598229738909171</v>
+        <v>1.362925872965921</v>
       </c>
       <c r="AH28" s="65">
         <f t="shared" si="13"/>
-        <v>1.5193994030941278</v>
+        <v>1.512408832821629</v>
       </c>
       <c r="AI28" s="47">
         <f t="shared" si="14"/>
-        <v>0.20140046473684037</v>
+        <v>0.19587296857154435</v>
       </c>
       <c r="AJ28" s="76">
         <f t="shared" si="15"/>
-        <v>1.3920448053201606</v>
+        <v>1.3885495201839113</v>
       </c>
       <c r="AT28" s="9"/>
       <c r="AZ28" s="1"/>
@@ -6541,27 +6542,27 @@
       </c>
       <c r="AE29" s="65">
         <f t="shared" si="10"/>
-        <v>1.2903578197754684</v>
+        <v>1.2957830949161677</v>
       </c>
       <c r="AF29" s="47">
         <f t="shared" si="11"/>
-        <v>6.7532429381873316E-2</v>
+        <v>7.2020841093923593E-2</v>
       </c>
       <c r="AG29" s="75">
         <f t="shared" si="12"/>
-        <v>1.2495436037652852</v>
+        <v>1.2522562413356348</v>
       </c>
       <c r="AH29" s="65">
         <f t="shared" si="13"/>
-        <v>1.5129993237057375</v>
+        <v>1.506038199413422</v>
       </c>
       <c r="AI29" s="47">
         <f t="shared" si="14"/>
-        <v>0.12194461297881731</v>
+        <v>0.11678268344079834</v>
       </c>
       <c r="AJ29" s="76">
         <f t="shared" si="15"/>
-        <v>1.4307750700161339</v>
+        <v>1.4272945078699761</v>
       </c>
       <c r="AT29" s="9"/>
       <c r="AW29" s="9"/>
@@ -6683,27 +6684,27 @@
       </c>
       <c r="AE30" s="65">
         <f t="shared" si="10"/>
-        <v>1.2822366156544678</v>
+        <v>1.2876277454083953</v>
       </c>
       <c r="AF30" s="47">
         <f t="shared" si="11"/>
-        <v>0.15192347769960102</v>
+        <v>0.14710052404935614</v>
       </c>
       <c r="AG30" s="75">
         <f t="shared" si="12"/>
-        <v>1.3796375385964645</v>
+        <v>1.3823331034734283</v>
       </c>
       <c r="AH30" s="65">
         <f t="shared" si="13"/>
-        <v>1.4918510270701912</v>
+        <v>1.4849872034964844</v>
       </c>
       <c r="AI30" s="47">
         <f t="shared" si="14"/>
-        <v>0.11059758902334393</v>
+        <v>0.1157309301689724</v>
       </c>
       <c r="AJ30" s="76">
         <f t="shared" si="15"/>
-        <v>1.5743485904581724</v>
+        <v>1.5709166786713191</v>
       </c>
       <c r="AT30" s="9"/>
       <c r="AZ30" s="1"/>
@@ -6824,27 +6825,27 @@
       </c>
       <c r="AE31" s="65">
         <f t="shared" si="10"/>
-        <v>1.4144670857905011</v>
+        <v>1.4204141750399095</v>
       </c>
       <c r="AF31" s="47">
         <f t="shared" si="11"/>
-        <v>0.17585982543143674</v>
+        <v>0.17093665340913677</v>
       </c>
       <c r="AG31" s="75">
         <f t="shared" si="12"/>
-        <v>1.5388410531833163</v>
+        <v>1.5418145978080204</v>
       </c>
       <c r="AH31" s="65">
         <f t="shared" si="13"/>
-        <v>1.4532585322797664</v>
+        <v>1.4465722680405397</v>
       </c>
       <c r="AI31" s="47">
         <f t="shared" si="14"/>
-        <v>0.1635870430440225</v>
+        <v>0.16896530903668605</v>
       </c>
       <c r="AJ31" s="76">
         <f t="shared" si="15"/>
-        <v>1.5721256653168378</v>
+        <v>1.5687825331972247</v>
       </c>
       <c r="AT31" s="9"/>
       <c r="AW31" s="9"/>
@@ -6966,27 +6967,27 @@
       </c>
       <c r="AE32" s="65">
         <f t="shared" si="10"/>
-        <v>1.1470354862150614</v>
+        <v>1.1518581664154615</v>
       </c>
       <c r="AF32" s="47">
         <f t="shared" si="11"/>
-        <v>6.2218274012235897E-2</v>
+        <v>5.7770904372513865E-2</v>
       </c>
       <c r="AG32" s="75">
         <f t="shared" si="12"/>
-        <v>1.1827187703066047</v>
+        <v>1.1851301104068048</v>
       </c>
       <c r="AH32" s="65">
         <f t="shared" si="13"/>
-        <v>1.1034836393796572</v>
+        <v>1.098406646516604</v>
       </c>
       <c r="AI32" s="47">
         <f t="shared" si="14"/>
-        <v>6.8230897333200424E-2</v>
+        <v>7.3168413560959156E-2</v>
       </c>
       <c r="AJ32" s="76">
         <f t="shared" si="15"/>
-        <v>1.141129478833347</v>
+        <v>1.1385909824018206</v>
       </c>
       <c r="AT32" s="9"/>
       <c r="AZ32" s="1"/>
@@ -7107,27 +7108,27 @@
       </c>
       <c r="AE33" s="65">
         <f t="shared" si="10"/>
-        <v>2.7473333437541183</v>
+        <v>2.7588844337422254</v>
       </c>
       <c r="AF33" s="47">
         <f t="shared" si="11"/>
-        <v>2.7851480091291236E-2</v>
+        <v>3.2173054307225391E-2</v>
       </c>
       <c r="AG33" s="75">
         <f t="shared" si="12"/>
-        <v>2.7101113805572017</v>
+        <v>2.7158869255512554</v>
       </c>
       <c r="AH33" s="65">
         <f t="shared" si="13"/>
-        <v>1.8262720417644012</v>
+        <v>1.8178695881247224</v>
       </c>
       <c r="AI33" s="47">
         <f t="shared" si="14"/>
-        <v>9.7342040598621837E-2</v>
+        <v>9.2293304478184623E-2</v>
       </c>
       <c r="AJ33" s="76">
         <f t="shared" si="15"/>
-        <v>1.7452703847347573</v>
+        <v>1.741069157914918</v>
       </c>
       <c r="AT33" s="9"/>
       <c r="AW33" s="9"/>
@@ -7249,27 +7250,27 @@
       </c>
       <c r="AE34" s="65">
         <f t="shared" si="10"/>
-        <v>1.0274995225678794</v>
+        <v>1.0318196169877649</v>
       </c>
       <c r="AF34" s="47">
         <f t="shared" si="11"/>
-        <v>9.9614078995184707E-2</v>
+        <v>9.5010137987973753E-2</v>
       </c>
       <c r="AG34" s="75">
         <f t="shared" si="12"/>
-        <v>1.078676231872175</v>
+        <v>1.0808362790821178</v>
       </c>
       <c r="AH34" s="65">
         <f t="shared" si="13"/>
-        <v>0.93321188868227234</v>
+        <v>0.92891829525734404</v>
       </c>
       <c r="AI34" s="47">
         <f t="shared" si="14"/>
-        <v>0.13192249501164244</v>
+        <v>0.13715440292746606</v>
       </c>
       <c r="AJ34" s="76">
         <f t="shared" si="15"/>
-        <v>0.99476770904701861</v>
+        <v>0.99262091233455441</v>
       </c>
       <c r="AT34" s="9"/>
       <c r="AW34" s="9"/>
@@ -7391,27 +7392,27 @@
       </c>
       <c r="AE35" s="65">
         <f t="shared" si="10"/>
-        <v>1.7855482410534744</v>
+        <v>1.7930555311525822</v>
       </c>
       <c r="AF35" s="47">
         <f t="shared" si="11"/>
-        <v>0.15749239275538773</v>
+        <v>0.15264612278273404</v>
       </c>
       <c r="AG35" s="75">
         <f t="shared" si="12"/>
-        <v>1.9261533734853171</v>
+        <v>1.929907018534871</v>
       </c>
       <c r="AH35" s="65">
         <f t="shared" si="13"/>
-        <v>1.3349542210379588</v>
+        <v>1.3288122604226453</v>
       </c>
       <c r="AI35" s="47">
         <f t="shared" si="14"/>
-        <v>0.16923041872299094</v>
+        <v>0.17463476920643606</v>
       </c>
       <c r="AJ35" s="76">
         <f t="shared" si="15"/>
-        <v>1.4479116519390978</v>
+        <v>1.444840671631441</v>
       </c>
       <c r="AT35" s="9"/>
       <c r="AZ35" s="1"/>
@@ -7532,27 +7533,27 @@
       </c>
       <c r="AE36" s="65">
         <f t="shared" si="10"/>
-        <v>1.4215451236977186</v>
+        <v>1.4275219723692922</v>
       </c>
       <c r="AF36" s="47">
         <f t="shared" si="11"/>
-        <v>5.2265426799740666E-2</v>
+        <v>5.6689648805406945E-2</v>
       </c>
       <c r="AG36" s="75">
         <f t="shared" si="12"/>
-        <v>1.3862414537714371</v>
+        <v>1.3892298781072241</v>
       </c>
       <c r="AH36" s="65">
         <f t="shared" si="13"/>
-        <v>1.4547955726889805</v>
+        <v>1.4481022367153764</v>
       </c>
       <c r="AI36" s="47">
         <f t="shared" si="14"/>
-        <v>6.4422303914512202E-2</v>
+        <v>5.9525027464372382E-2</v>
       </c>
       <c r="AJ36" s="76">
         <f t="shared" si="15"/>
-        <v>1.410771090031774</v>
+        <v>1.4074244220449721</v>
       </c>
       <c r="AT36" s="9"/>
       <c r="AZ36" s="1"/>
@@ -7673,27 +7674,27 @@
       </c>
       <c r="AE37" s="65">
         <f t="shared" si="10"/>
-        <v>2.1245658597222565</v>
+        <v>2.1334985403840716</v>
       </c>
       <c r="AF37" s="47">
         <f t="shared" si="11"/>
-        <v>7.3720814456186279E-3</v>
+        <v>1.1607550574524783E-2</v>
       </c>
       <c r="AG37" s="75">
         <f t="shared" si="12"/>
-        <v>2.1167919334625687</v>
+        <v>2.121258273793476</v>
       </c>
       <c r="AH37" s="65">
         <f t="shared" si="13"/>
-        <v>1.2129673588364496</v>
+        <v>1.2073866448102848</v>
       </c>
       <c r="AI37" s="47">
         <f t="shared" si="14"/>
-        <v>4.3117935520211814E-2</v>
+        <v>4.793937604112819E-2</v>
       </c>
       <c r="AJ37" s="76">
         <f t="shared" si="15"/>
-        <v>1.2391176830196655</v>
+        <v>1.236327326006583</v>
       </c>
       <c r="AT37" s="9"/>
       <c r="AZ37" s="1"/>
@@ -7869,27 +7870,27 @@
       </c>
       <c r="AE39" s="65">
         <f t="shared" si="10"/>
-        <v>2.0559538837673372</v>
+        <v>2.0645980872007446</v>
       </c>
       <c r="AF39" s="47">
         <f t="shared" si="11"/>
-        <v>0.12736447704402676</v>
+        <v>0.12264434873257501</v>
       </c>
       <c r="AG39" s="75">
         <f t="shared" si="12"/>
-        <v>2.1868816293836684</v>
+        <v>2.191203731100372</v>
       </c>
       <c r="AH39" s="65">
         <f t="shared" si="13"/>
-        <v>1.3140619570493324</v>
+        <v>1.3080161191778259</v>
       </c>
       <c r="AI39" s="47">
         <f t="shared" si="14"/>
-        <v>0.13281616366290971</v>
+        <v>0.13805220224325443</v>
       </c>
       <c r="AJ39" s="76">
         <f t="shared" si="15"/>
-        <v>1.4013262910246662</v>
+        <v>1.3983033720889129</v>
       </c>
       <c r="AT39" s="9"/>
       <c r="AZ39" s="1"/>
@@ -8010,27 +8011,27 @@
       </c>
       <c r="AE40" s="65">
         <f t="shared" si="10"/>
-        <v>1.3421126623215807</v>
+        <v>1.3477555393215266</v>
       </c>
       <c r="AF40" s="47">
         <f t="shared" si="11"/>
-        <v>0.14249397093556593</v>
+        <v>0.14729755645573928</v>
       </c>
       <c r="AG40" s="75">
         <f t="shared" si="12"/>
-        <v>1.2584172698021343</v>
+        <v>1.2612387083021073</v>
       </c>
       <c r="AH40" s="65">
         <f t="shared" si="13"/>
-        <v>1.6706351645134025</v>
+        <v>1.6629487770543472</v>
       </c>
       <c r="AI40" s="47">
         <f t="shared" si="14"/>
-        <v>0.19096088067846306</v>
+        <v>0.18548141575882049</v>
       </c>
       <c r="AJ40" s="76">
         <f t="shared" si="15"/>
-        <v>1.5366987911683156</v>
+        <v>1.5328555974387879</v>
       </c>
       <c r="AT40" s="9"/>
       <c r="AZ40" s="1"/>
@@ -8151,27 +8152,27 @@
       </c>
       <c r="AE41" s="65">
         <f t="shared" si="10"/>
-        <v>0.96951054225976407</v>
+        <v>0.97358682355395831</v>
       </c>
       <c r="AF41" s="47">
         <f t="shared" si="11"/>
-        <v>4.4834374689099787E-2</v>
+        <v>4.0459789172905936E-2</v>
       </c>
       <c r="AG41" s="75">
         <f t="shared" si="12"/>
-        <v>0.99124424171811731</v>
+        <v>0.99328238236521438</v>
       </c>
       <c r="AH41" s="65">
         <f t="shared" si="13"/>
-        <v>3.1800158392030604</v>
+        <v>3.1653849764119215</v>
       </c>
       <c r="AI41" s="47">
         <f t="shared" si="14"/>
-        <v>4.4991095430176209E-2</v>
+        <v>4.9821193964519894E-2</v>
       </c>
       <c r="AJ41" s="76">
         <f t="shared" si="15"/>
-        <v>3.2515520372485889</v>
+        <v>3.2442366058530192</v>
       </c>
       <c r="AT41" s="9"/>
       <c r="AW41" s="9"/>
@@ -8293,27 +8294,27 @@
       </c>
       <c r="AE42" s="65">
         <f t="shared" si="10"/>
-        <v>1.587295091584541</v>
+        <v>1.593968831588555</v>
       </c>
       <c r="AF42" s="47">
         <f t="shared" si="11"/>
-        <v>4.4475196343974455E-2</v>
+        <v>4.0102114660755861E-2</v>
       </c>
       <c r="AG42" s="75">
         <f t="shared" si="12"/>
-        <v>1.6225927220115657</v>
+        <v>1.6259295920135726</v>
       </c>
       <c r="AH42" s="65">
         <f t="shared" si="13"/>
-        <v>1.9395545442781825</v>
+        <v>1.9306308917405348</v>
       </c>
       <c r="AI42" s="47">
         <f t="shared" si="14"/>
-        <v>3.1523945595841374E-2</v>
+        <v>3.6291797034529338E-2</v>
       </c>
       <c r="AJ42" s="76">
         <f t="shared" si="15"/>
-        <v>1.9701257502451788</v>
+        <v>1.9656639239763547</v>
       </c>
       <c r="AT42" s="9"/>
       <c r="AW42" s="9"/>
@@ -8435,27 +8436,27 @@
       </c>
       <c r="AE43" s="65">
         <f t="shared" si="10"/>
-        <v>1.7392217813768776</v>
+        <v>1.7465342931081651</v>
       </c>
       <c r="AF43" s="47">
         <f t="shared" si="11"/>
-        <v>0.36407701909048562</v>
+        <v>0.36981224464440121</v>
       </c>
       <c r="AG43" s="75">
         <f t="shared" si="12"/>
-        <v>1.507119534641888</v>
+        <v>1.5107757905075316</v>
       </c>
       <c r="AH43" s="65">
         <f t="shared" si="13"/>
-        <v>1.8025363362990687</v>
+        <v>1.7942430877286328</v>
       </c>
       <c r="AI43" s="47">
         <f t="shared" si="14"/>
-        <v>0.37871447289546034</v>
+        <v>0.37237117672931719</v>
       </c>
       <c r="AJ43" s="76">
         <f t="shared" si="15"/>
-        <v>1.5549699939211654</v>
+        <v>1.5508233696359475</v>
       </c>
       <c r="AT43" s="9"/>
       <c r="AZ43" s="1"/>
@@ -8576,27 +8577,27 @@
       </c>
       <c r="AE44" s="65">
         <f t="shared" si="10"/>
-        <v>1.5654398505325171</v>
+        <v>1.5720217007566915</v>
       </c>
       <c r="AF44" s="47">
         <f t="shared" si="11"/>
-        <v>4.9961963476177429E-2</v>
+        <v>4.5565909413212591E-2</v>
       </c>
       <c r="AG44" s="75">
         <f t="shared" si="12"/>
-        <v>1.6045460748507461</v>
+        <v>1.6078369999628332</v>
       </c>
       <c r="AH44" s="65">
         <f t="shared" si="13"/>
-        <v>1.6166794717006083</v>
+        <v>1.6092413277655673</v>
       </c>
       <c r="AI44" s="47">
         <f t="shared" si="14"/>
-        <v>4.6309466793512222E-2</v>
+        <v>5.1145659029149249E-2</v>
       </c>
       <c r="AJ44" s="76">
         <f t="shared" si="15"/>
-        <v>1.6541132538558445</v>
+        <v>1.6503941818883239</v>
       </c>
       <c r="AT44" s="9"/>
       <c r="AZ44" s="1"/>
@@ -8717,27 +8718,27 @@
       </c>
       <c r="AE45" s="65">
         <f t="shared" si="10"/>
-        <v>1.5882489913321929</v>
+        <v>1.5949267419823301</v>
       </c>
       <c r="AF45" s="47">
         <f t="shared" si="11"/>
-        <v>6.7478977247043881E-2</v>
+        <v>7.1967164221014679E-2</v>
       </c>
       <c r="AG45" s="75">
         <f t="shared" si="12"/>
-        <v>1.5380496806979269</v>
+        <v>1.5413885560229956</v>
       </c>
       <c r="AH45" s="65">
         <f t="shared" si="13"/>
-        <v>1.6376997480936273</v>
+        <v>1.6301648924454095</v>
       </c>
       <c r="AI45" s="47">
         <f t="shared" si="14"/>
-        <v>7.9701983964263423E-2</v>
+        <v>7.4734407580536732E-2</v>
       </c>
       <c r="AJ45" s="76">
         <f t="shared" si="15"/>
-        <v>1.5772534763448312</v>
+        <v>1.5734860485207223</v>
       </c>
       <c r="AT45" s="9"/>
       <c r="AZ45" s="1"/>
@@ -8858,27 +8859,27 @@
       </c>
       <c r="AE46" s="65">
         <f t="shared" si="10"/>
-        <v>3.3029693343656046</v>
+        <v>3.3168565811010442</v>
       </c>
       <c r="AF46" s="47">
         <f t="shared" si="11"/>
-        <v>1.1352238821794813E-2</v>
+        <v>7.1178386499624047E-3</v>
       </c>
       <c r="AG46" s="75">
         <f t="shared" si="12"/>
-        <v>3.321717382717996</v>
+        <v>3.3286610060857158</v>
       </c>
       <c r="AH46" s="65">
         <f t="shared" si="13"/>
-        <v>0.93637409165710617</v>
+        <v>0.93206594932419051</v>
       </c>
       <c r="AI46" s="47">
         <f t="shared" si="14"/>
-        <v>3.1324295010735081E-3</v>
+        <v>1.4850618936907978E-3</v>
       </c>
       <c r="AJ46" s="76">
         <f t="shared" si="15"/>
-        <v>0.93491210830252236</v>
+        <v>0.93275803713606453</v>
       </c>
       <c r="AT46" s="9"/>
       <c r="AW46" s="9"/>
@@ -9000,27 +9001,27 @@
       </c>
       <c r="AE47" s="65">
         <f t="shared" si="10"/>
-        <v>1.8753700275698835</v>
+        <v>1.8832549709819042</v>
       </c>
       <c r="AF47" s="47">
         <f t="shared" si="11"/>
-        <v>4.4138162370356948E-2</v>
+        <v>4.8528213508846063E-2</v>
       </c>
       <c r="AG47" s="75">
         <f t="shared" si="12"/>
-        <v>1.8357318887849419</v>
+        <v>1.8396743604909522</v>
       </c>
       <c r="AH47" s="65">
         <f t="shared" si="13"/>
-        <v>1.5542077782274208</v>
+        <v>1.5470570588907948</v>
       </c>
       <c r="AI47" s="47">
         <f t="shared" si="14"/>
-        <v>3.9047310116131939E-2</v>
+        <v>3.4266780899767646E-2</v>
       </c>
       <c r="AJ47" s="76">
         <f t="shared" si="15"/>
-        <v>1.5250042797387104</v>
+        <v>1.5214289200703974</v>
       </c>
       <c r="AT47" s="9"/>
       <c r="AZ47" s="1"/>
@@ -9195,27 +9196,27 @@
       </c>
       <c r="AE49" s="65">
         <f t="shared" si="10"/>
-        <v>1.9029472905240703</v>
+        <v>1.910948181804861</v>
       </c>
       <c r="AF49" s="47">
         <f t="shared" si="11"/>
-        <v>0.23949450575454567</v>
+        <v>0.24470592744397579</v>
       </c>
       <c r="AG49" s="75">
         <f t="shared" si="12"/>
-        <v>1.7191040307495635</v>
+        <v>1.7231044763899588</v>
       </c>
       <c r="AH49" s="65">
         <f t="shared" si="13"/>
-        <v>1.8910884810833399</v>
+        <v>1.882387814957234</v>
       </c>
       <c r="AI49" s="47">
         <f t="shared" si="14"/>
-        <v>0.25004874489657913</v>
+        <v>0.24429742396183762</v>
       </c>
       <c r="AJ49" s="76">
         <f t="shared" si="15"/>
-        <v>1.7019501362332801</v>
+        <v>1.6975998031702271</v>
       </c>
       <c r="AT49" s="9"/>
       <c r="AW49" s="9"/>
@@ -9337,27 +9338,27 @@
       </c>
       <c r="AE50" s="65">
         <f t="shared" si="10"/>
-        <v>1.4973428663379782</v>
+        <v>1.5036384046029074</v>
       </c>
       <c r="AF50" s="47">
         <f t="shared" si="11"/>
-        <v>8.6696760794943151E-2</v>
+        <v>8.2146902917532794E-2</v>
       </c>
       <c r="AG50" s="75">
         <f t="shared" si="12"/>
-        <v>1.5622502544934371</v>
+        <v>1.5653980236259017</v>
       </c>
       <c r="AH50" s="65">
         <f t="shared" si="13"/>
-        <v>1.507001889580551</v>
+        <v>1.5000683587469543</v>
       </c>
       <c r="AI50" s="47">
         <f t="shared" si="14"/>
-        <v>7.7531041829186575E-2</v>
+        <v>8.2511544657018598E-2</v>
       </c>
       <c r="AJ50" s="76">
         <f t="shared" si="15"/>
-        <v>1.5654216028494177</v>
+        <v>1.5619548374326193</v>
       </c>
       <c r="AT50" s="9"/>
       <c r="AZ50" s="1"/>
@@ -9478,27 +9479,27 @@
       </c>
       <c r="AE51" s="65">
         <f t="shared" si="10"/>
-        <v>1.9597480694489353</v>
+        <v>1.9679877780942976</v>
       </c>
       <c r="AF51" s="47">
         <f t="shared" si="11"/>
-        <v>5.6616999542325797E-2</v>
+        <v>5.2193081709667188E-2</v>
       </c>
       <c r="AG51" s="75">
         <f t="shared" si="12"/>
-        <v>2.0152255972244673</v>
+        <v>2.0193454515471485</v>
       </c>
       <c r="AH51" s="65">
         <f t="shared" si="13"/>
-        <v>1.4498616729754037</v>
+        <v>1.4431910372691519</v>
       </c>
       <c r="AI51" s="47">
         <f t="shared" si="14"/>
-        <v>5.9637725195638813E-2</v>
+        <v>6.4535522550836166E-2</v>
       </c>
       <c r="AJ51" s="76">
         <f t="shared" si="15"/>
-        <v>1.4930948989877018</v>
+        <v>1.4897595811345758</v>
       </c>
       <c r="AT51" s="9"/>
       <c r="AZ51" s="1"/>
@@ -9619,27 +9620,27 @@
       </c>
       <c r="AE52" s="65">
         <f t="shared" si="10"/>
-        <v>1.6297829115436129</v>
+        <v>1.6366352904568302</v>
       </c>
       <c r="AF52" s="47">
         <f t="shared" si="11"/>
-        <v>8.606857221210551E-2</v>
+        <v>8.1521344478517443E-2</v>
       </c>
       <c r="AG52" s="75">
         <f t="shared" si="12"/>
-        <v>1.6999194556497363</v>
+        <v>1.7033456451063449</v>
       </c>
       <c r="AH52" s="65">
         <f t="shared" si="13"/>
-        <v>1.8460273883700258</v>
+        <v>1.8375340428039559</v>
       </c>
       <c r="AI52" s="47">
         <f t="shared" si="14"/>
-        <v>7.37332355851541E-2</v>
+        <v>7.86961844085039E-2</v>
       </c>
       <c r="AJ52" s="76">
         <f t="shared" si="15"/>
-        <v>1.9140841745316928</v>
+        <v>1.9098375017486577</v>
       </c>
       <c r="AT52" s="9"/>
       <c r="AZ52" s="1"/>
@@ -9760,27 +9761,27 @@
       </c>
       <c r="AE53" s="65">
         <f t="shared" si="10"/>
-        <v>1.2377457873464626</v>
+        <v>1.2429498565958468</v>
       </c>
       <c r="AF53" s="47">
         <f t="shared" si="11"/>
-        <v>3.9858724352422215E-2</v>
+        <v>3.5504971236486327E-2</v>
       </c>
       <c r="AG53" s="75">
         <f t="shared" si="12"/>
-        <v>1.2624132714245699</v>
+        <v>1.2650153060492619</v>
       </c>
       <c r="AH53" s="65">
         <f t="shared" si="13"/>
-        <v>1.0215178057394398</v>
+        <v>1.0168179276224099</v>
       </c>
       <c r="AI53" s="47">
         <f t="shared" si="14"/>
-        <v>9.3878261424409137E-2</v>
+        <v>9.8934323442891436E-2</v>
       </c>
       <c r="AJ53" s="76">
         <f t="shared" si="15"/>
-        <v>1.0694669635478879</v>
+        <v>1.0671170244893728</v>
       </c>
       <c r="AT53" s="9"/>
       <c r="AW53" s="9"/>
@@ -9902,27 +9903,27 @@
       </c>
       <c r="AE54" s="65">
         <f t="shared" si="10"/>
-        <v>1.9540733780693864</v>
+        <v>1.962289227625742</v>
       </c>
       <c r="AF54" s="47">
         <f t="shared" si="11"/>
-        <v>0.1147278763174211</v>
+        <v>0.11941472003111442</v>
       </c>
       <c r="AG54" s="75">
         <f t="shared" si="12"/>
-        <v>1.8535166890346932</v>
+        <v>1.8576246138128709</v>
       </c>
       <c r="AH54" s="65">
         <f t="shared" si="13"/>
-        <v>0.79975381722343886</v>
+        <v>0.79607424801430615</v>
       </c>
       <c r="AI54" s="47">
         <f t="shared" si="14"/>
-        <v>0.11081266201505113</v>
+        <v>0.11594699725885604</v>
       </c>
       <c r="AJ54" s="76">
         <f t="shared" si="15"/>
-        <v>0.84406524194505284</v>
+        <v>0.84222545734048648</v>
       </c>
       <c r="AT54" s="9"/>
       <c r="AW54" s="9"/>
@@ -10044,27 +10045,27 @@
       </c>
       <c r="AE55" s="65">
         <f t="shared" si="10"/>
-        <v>2.003899406852963</v>
+        <v>2.0123247486223907</v>
       </c>
       <c r="AF55" s="47">
         <f t="shared" si="11"/>
-        <v>8.4838899659995359E-2</v>
+        <v>8.0296820405311164E-2</v>
       </c>
       <c r="AG55" s="75">
         <f t="shared" si="12"/>
-        <v>2.0889037172063243</v>
+        <v>2.0931163880910382</v>
       </c>
       <c r="AH55" s="65">
         <f t="shared" si="13"/>
-        <v>1.4565859329225992</v>
+        <v>1.4498843597211795</v>
       </c>
       <c r="AI55" s="47">
         <f t="shared" si="14"/>
-        <v>9.2386536927564267E-2</v>
+        <v>9.7435703981737731E-2</v>
       </c>
       <c r="AJ55" s="76">
         <f t="shared" si="15"/>
-        <v>1.5238703979626615</v>
+        <v>1.5205196113619515</v>
       </c>
       <c r="AT55" s="9"/>
       <c r="AW55" s="9"/>
@@ -10186,27 +10187,27 @@
       </c>
       <c r="AE56" s="65">
         <f t="shared" si="10"/>
-        <v>1.3515503927234034</v>
+        <v>1.3572329504098604</v>
       </c>
       <c r="AF56" s="47">
         <f t="shared" si="11"/>
-        <v>2.767881837942765E-2</v>
+        <v>3.1999666643785396E-2</v>
       </c>
       <c r="AG56" s="75">
         <f t="shared" si="12"/>
-        <v>1.3333495126518327</v>
+        <v>1.336190791495061</v>
       </c>
       <c r="AH56" s="65">
         <f t="shared" si="13"/>
-        <v>2.1846400547863443</v>
+        <v>2.1745887938789097</v>
       </c>
       <c r="AI56" s="47">
         <f t="shared" si="14"/>
-        <v>5.3135045007334902E-2</v>
+        <v>4.8289699850845524E-2</v>
       </c>
       <c r="AJ56" s="76">
         <f t="shared" si="15"/>
-        <v>2.1295279643729583</v>
+        <v>2.1245023339192413</v>
       </c>
       <c r="AT56" s="9"/>
       <c r="AZ56" s="1"/>
@@ -10327,27 +10328,27 @@
       </c>
       <c r="AE57" s="65">
         <f t="shared" si="10"/>
-        <v>1.741850036203171</v>
+        <v>1.7491735983619865</v>
       </c>
       <c r="AF57" s="47">
         <f t="shared" si="11"/>
-        <v>6.8794288508192025E-2</v>
+        <v>7.3288005673384005E-2</v>
       </c>
       <c r="AG57" s="75">
         <f t="shared" si="12"/>
-        <v>1.6857918521274393</v>
+        <v>1.6894536332068473</v>
       </c>
       <c r="AH57" s="65">
         <f t="shared" si="13"/>
-        <v>1.8625481768867831</v>
+        <v>1.8539788211993138</v>
       </c>
       <c r="AI57" s="47">
         <f t="shared" si="14"/>
-        <v>8.4603965126985869E-2</v>
+        <v>7.9613835329243932E-2</v>
       </c>
       <c r="AJ57" s="76">
         <f t="shared" si="15"/>
-        <v>1.7899046286095963</v>
+        <v>1.7856199507658617</v>
       </c>
       <c r="AT57" s="9"/>
       <c r="AZ57" s="1"/>
@@ -10468,27 +10469,27 @@
       </c>
       <c r="AE58" s="65">
         <f t="shared" si="10"/>
-        <v>1.066534050365644</v>
+        <v>1.0710182644196689</v>
       </c>
       <c r="AF58" s="47">
         <f t="shared" si="11"/>
-        <v>0.10647606669200149</v>
+        <v>0.10184339543555843</v>
       </c>
       <c r="AG58" s="75">
         <f t="shared" si="12"/>
-        <v>1.1233142257036555</v>
+        <v>1.1255563327306679</v>
       </c>
       <c r="AH58" s="65">
         <f t="shared" si="13"/>
-        <v>1.5421699766114254</v>
+        <v>1.5350746417233858</v>
       </c>
       <c r="AI58" s="47">
         <f t="shared" si="14"/>
-        <v>7.1141959684291045E-3</v>
+        <v>1.1769222047729233E-2</v>
       </c>
       <c r="AJ58" s="76">
         <f t="shared" si="15"/>
-        <v>1.547655626326546</v>
+        <v>1.5441079588825262</v>
       </c>
       <c r="AT58" s="9"/>
       <c r="AZ58" s="1"/>
@@ -10609,27 +10610,27 @@
       </c>
       <c r="AE59" s="65">
         <f t="shared" si="10"/>
-        <v>1.2382676389812743</v>
+        <v>1.2434739023419803</v>
       </c>
       <c r="AF59" s="47">
         <f t="shared" si="11"/>
-        <v>0.10443582667553608</v>
+        <v>9.9811697638455321E-2</v>
       </c>
       <c r="AG59" s="75">
         <f t="shared" si="12"/>
-        <v>1.3029273912425612</v>
+        <v>1.3055305229229142</v>
       </c>
       <c r="AH59" s="65">
         <f t="shared" si="13"/>
-        <v>1.8175746709804776</v>
+        <v>1.8092122328768894</v>
       </c>
       <c r="AI59" s="47">
         <f t="shared" si="14"/>
-        <v>3.0442557515225843E-2</v>
+        <v>3.5205410623300404E-2</v>
       </c>
       <c r="AJ59" s="76">
         <f t="shared" si="15"/>
-        <v>1.8452404817102481</v>
+        <v>1.8410592626584539</v>
       </c>
       <c r="AT59" s="9"/>
       <c r="AW59" s="9"/>
@@ -10751,27 +10752,27 @@
       </c>
       <c r="AE60" s="65">
         <f t="shared" si="10"/>
-        <v>2.1978414712663681</v>
+        <v>2.2070822372884114</v>
       </c>
       <c r="AF60" s="47">
         <f t="shared" si="11"/>
-        <v>0.11212235181585761</v>
+        <v>0.11679824067106859</v>
       </c>
       <c r="AG60" s="75">
         <f t="shared" si="12"/>
-        <v>2.0870500847456102</v>
+        <v>2.0916704677566318</v>
       </c>
       <c r="AH60" s="65">
         <f t="shared" si="13"/>
-        <v>0.92491281634353784</v>
+        <v>0.92065740593241252</v>
       </c>
       <c r="AI60" s="47">
         <f t="shared" si="14"/>
-        <v>4.3454945176735205E-2</v>
+        <v>4.8277943404559487E-2</v>
       </c>
       <c r="AJ60" s="76">
         <f t="shared" si="15"/>
-        <v>0.945008834207272</v>
+        <v>0.94288112900170928</v>
       </c>
       <c r="AT60" s="9"/>
       <c r="AW60" s="9"/>
@@ -10893,27 +10894,27 @@
       </c>
       <c r="AE61" s="65">
         <f t="shared" si="10"/>
-        <v>1.5675081225118224</v>
+        <v>1.5740986687305352</v>
       </c>
       <c r="AF61" s="47">
         <f t="shared" si="11"/>
-        <v>0.43474403537371464</v>
+        <v>0.44077637851845108</v>
       </c>
       <c r="AG61" s="75">
         <f t="shared" si="12"/>
-        <v>1.3300215779225777</v>
+        <v>1.3333168510319342</v>
       </c>
       <c r="AH61" s="65">
         <f t="shared" si="13"/>
-        <v>1.9773770008599894</v>
+        <v>1.9682793318392002</v>
       </c>
       <c r="AI61" s="47">
         <f t="shared" si="14"/>
-        <v>0.4586307336494766</v>
+        <v>0.45191975257074324</v>
       </c>
       <c r="AJ61" s="76">
         <f t="shared" si="15"/>
-        <v>1.6665081004299946</v>
+        <v>1.6619592659196001</v>
       </c>
       <c r="AT61" s="9"/>
       <c r="AW61" s="9"/>
@@ -11035,27 +11036,27 @@
       </c>
       <c r="AE62" s="65">
         <f t="shared" si="10"/>
-        <v>1.9161981123500698</v>
+        <v>1.9242547163588688</v>
       </c>
       <c r="AF62" s="47">
         <f t="shared" si="11"/>
-        <v>0.1330827739943532</v>
+        <v>0.12833870391794577</v>
       </c>
       <c r="AG62" s="75">
         <f t="shared" si="12"/>
-        <v>2.0437045925072148</v>
+        <v>2.0477328945116144</v>
       </c>
       <c r="AH62" s="65">
         <f t="shared" si="13"/>
-        <v>1.1991725780046119</v>
+        <v>1.1936553320728811</v>
       </c>
       <c r="AI62" s="47">
         <f t="shared" si="14"/>
-        <v>0.15756719494039628</v>
+        <v>0.1629176363328031</v>
       </c>
       <c r="AJ62" s="76">
         <f t="shared" si="15"/>
-        <v>1.2936477076874269</v>
+        <v>1.2908890847215617</v>
       </c>
       <c r="AT62" s="9"/>
       <c r="AW62" s="9"/>
@@ -11177,27 +11178,27 @@
       </c>
       <c r="AE63" s="65">
         <f t="shared" si="10"/>
-        <v>1.5433049039302107</v>
+        <v>1.549793688359997</v>
       </c>
       <c r="AF63" s="47">
         <f t="shared" si="11"/>
-        <v>0.13045710899840057</v>
+        <v>0.12572403223953721</v>
       </c>
       <c r="AG63" s="75">
         <f t="shared" si="12"/>
-        <v>1.6439724519651056</v>
+        <v>1.6472168441799986</v>
       </c>
       <c r="AH63" s="65">
         <f t="shared" si="13"/>
-        <v>1.6178805371898164</v>
+        <v>1.6104368672997915</v>
       </c>
       <c r="AI63" s="47">
         <f t="shared" si="14"/>
-        <v>0.11852510639831371</v>
+        <v>0.12369508966483811</v>
       </c>
       <c r="AJ63" s="76">
         <f t="shared" si="15"/>
-        <v>1.7137602685949083</v>
+        <v>1.7100384336498959</v>
       </c>
       <c r="AT63" s="9"/>
       <c r="AZ63" s="1"/>
@@ -11294,27 +11295,27 @@
       </c>
       <c r="AE64" s="65">
         <f t="shared" si="10"/>
-        <v>1.5143895955163331</v>
+        <v>1.5207568063007946</v>
       </c>
       <c r="AF64" s="47">
         <f t="shared" si="11"/>
-        <v>0.10060674596487229</v>
+        <v>9.599864879027864E-2</v>
       </c>
       <c r="AG64" s="75">
         <f t="shared" si="12"/>
-        <v>1.5905685001803118</v>
+        <v>1.5937521055725425</v>
       </c>
       <c r="AH64" s="65">
         <f t="shared" si="13"/>
-        <v>1.8723757833682251</v>
+        <v>1.863761212068864</v>
       </c>
       <c r="AI64" s="47">
         <f t="shared" si="14"/>
-        <v>8.6531070172323421E-2</v>
+        <v>9.1553172420379303E-2</v>
       </c>
       <c r="AJ64" s="76">
         <f t="shared" si="15"/>
-        <v>1.9533851235180224</v>
+        <v>1.949077837868342</v>
       </c>
       <c r="AT64" s="9"/>
       <c r="AW64" s="9"/>
@@ -11335,21 +11336,15 @@
         <v>70</v>
       </c>
       <c r="AA66" s="73">
-        <f>AVERAGE(AA2:AA64)</f>
-        <v>1.7003405984755176</v>
-      </c>
-      <c r="AB66" s="73">
-        <f t="shared" ref="AB66:AD66" si="46">AVERAGE(AB2:AB64)</f>
-        <v>1.5538420860304829</v>
-      </c>
+        <f>AVERAGE(AA2:AB64)</f>
+        <v>1.6270913422530002</v>
+      </c>
+      <c r="AB66" s="73"/>
       <c r="AC66" s="73">
-        <f t="shared" si="46"/>
-        <v>2.1473897828154294</v>
-      </c>
-      <c r="AD66" s="73">
-        <f t="shared" si="46"/>
-        <v>1.9451672105778679</v>
-      </c>
+        <f>AVERAGE(AC2:AD64)</f>
+        <v>2.0462784966966479</v>
+      </c>
+      <c r="AD66" s="73"/>
       <c r="AZ66" s="1"/>
       <c r="BA66" s="1"/>
       <c r="BB66" s="1"/>
@@ -19419,4 +19414,1326 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E64"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G23" sqref="G23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="2" width="17.83203125" customWidth="1"/>
+    <col min="4" max="5" width="10.83203125" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" t="str">
+        <f>DistanserMerge!A1</f>
+        <v>A</v>
+      </c>
+      <c r="B1" t="str">
+        <f>DistanserMerge!B1</f>
+        <v>B</v>
+      </c>
+      <c r="C1" t="str">
+        <f>DistanserMerge!F1</f>
+        <v>Distanse</v>
+      </c>
+      <c r="D1" s="1" t="str">
+        <f>DistanserMerge!AG1</f>
+        <v>TurFaktor</v>
+      </c>
+      <c r="E1" s="1" t="str">
+        <f>DistanserMerge!AJ1</f>
+        <v>ReturFaktor</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" t="str">
+        <f>DistanserMerge!A2</f>
+        <v>Sognsvann</v>
+      </c>
+      <c r="B2" t="str">
+        <f>DistanserMerge!B2</f>
+        <v>Ullevålseter</v>
+      </c>
+      <c r="C2">
+        <f>DistanserMerge!F2</f>
+        <v>5.15</v>
+      </c>
+      <c r="D2" s="1">
+        <f>DistanserMerge!AG2</f>
+        <v>1.7502628643941507</v>
+      </c>
+      <c r="E2" s="1">
+        <f>DistanserMerge!AJ2</f>
+        <v>0.8572596088871296</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" t="str">
+        <f>DistanserMerge!A3</f>
+        <v>Sognsvann</v>
+      </c>
+      <c r="B3" t="str">
+        <f>DistanserMerge!B3</f>
+        <v>Sæteren</v>
+      </c>
+      <c r="C3">
+        <f>DistanserMerge!F3</f>
+        <v>13.35</v>
+      </c>
+      <c r="D3" s="1">
+        <f>DistanserMerge!AG3</f>
+        <v>1.2011190903267912</v>
+      </c>
+      <c r="E3" s="1">
+        <f>DistanserMerge!AJ3</f>
+        <v>1.2608280652671171</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" t="str">
+        <f>DistanserMerge!A4</f>
+        <v>Sognsvann</v>
+      </c>
+      <c r="B4" t="str">
+        <f>DistanserMerge!B4</f>
+        <v>Skjennungstua</v>
+      </c>
+      <c r="C4">
+        <f>DistanserMerge!F4</f>
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="D4" s="1">
+        <f>DistanserMerge!AG4</f>
+        <v>2.5109590627184972</v>
+      </c>
+      <c r="E4" s="1">
+        <f>DistanserMerge!AJ4</f>
+        <v>0.79104348735905128</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" t="str">
+        <f>DistanserMerge!A6</f>
+        <v>Ullevålseter</v>
+      </c>
+      <c r="B6" t="str">
+        <f>DistanserMerge!B6</f>
+        <v>Skjennungstua</v>
+      </c>
+      <c r="C6">
+        <f>DistanserMerge!F6</f>
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="D6" s="1">
+        <f>DistanserMerge!AG6</f>
+        <v>2.4379508533089091</v>
+      </c>
+      <c r="E6" s="1">
+        <f>DistanserMerge!AJ6</f>
+        <v>0.67891753308086877</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" t="str">
+        <f>DistanserMerge!A8</f>
+        <v>Ullevålseter</v>
+      </c>
+      <c r="B8" t="str">
+        <f>DistanserMerge!B8</f>
+        <v>Fagervann</v>
+      </c>
+      <c r="C8">
+        <f>DistanserMerge!F8</f>
+        <v>3.8499999999999996</v>
+      </c>
+      <c r="D8" s="1">
+        <f>DistanserMerge!AG8</f>
+        <v>2.3946456591823688</v>
+      </c>
+      <c r="E8" s="1">
+        <f>DistanserMerge!AJ8</f>
+        <v>1.612289567822295</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" t="str">
+        <f>DistanserMerge!A9</f>
+        <v>Ullevålseter</v>
+      </c>
+      <c r="B9" t="str">
+        <f>DistanserMerge!B9</f>
+        <v>Studenterhytta</v>
+      </c>
+      <c r="C9">
+        <f>DistanserMerge!F9</f>
+        <v>4.3499999999999996</v>
+      </c>
+      <c r="D9" s="1">
+        <f>DistanserMerge!AG9</f>
+        <v>1.4387457831489774</v>
+      </c>
+      <c r="E9" s="1">
+        <f>DistanserMerge!AJ9</f>
+        <v>1.1210566401268056</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" t="str">
+        <f>DistanserMerge!A11</f>
+        <v>Skjennungstua</v>
+      </c>
+      <c r="B11" t="str">
+        <f>DistanserMerge!B11</f>
+        <v>Studenterhytta</v>
+      </c>
+      <c r="C11">
+        <f>DistanserMerge!F11</f>
+        <v>3.8</v>
+      </c>
+      <c r="D11" s="1">
+        <f>DistanserMerge!AG11</f>
+        <v>1.1008921809362264</v>
+      </c>
+      <c r="E11" s="1">
+        <f>DistanserMerge!AJ11</f>
+        <v>1.757659220630845</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" t="str">
+        <f>DistanserMerge!A12</f>
+        <v>Skjennungstua</v>
+      </c>
+      <c r="B12" t="str">
+        <f>DistanserMerge!B12</f>
+        <v>Brunkollen</v>
+      </c>
+      <c r="C12">
+        <f>DistanserMerge!F12</f>
+        <v>13.7</v>
+      </c>
+      <c r="D12" s="1">
+        <f>DistanserMerge!AG12</f>
+        <v>1.4334301843390631</v>
+      </c>
+      <c r="E12" s="1">
+        <f>DistanserMerge!AJ12</f>
+        <v>1.6374927508164361</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" t="str">
+        <f>DistanserMerge!A13</f>
+        <v>Skjennungstua</v>
+      </c>
+      <c r="B13" t="str">
+        <f>DistanserMerge!B13</f>
+        <v>Sæteren</v>
+      </c>
+      <c r="C13">
+        <f>DistanserMerge!F13</f>
+        <v>14.1</v>
+      </c>
+      <c r="D13" s="1">
+        <f>DistanserMerge!AG13</f>
+        <v>1.17584191271765</v>
+      </c>
+      <c r="E13" s="1">
+        <f>DistanserMerge!AJ13</f>
+        <v>1.8471087732970077</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" t="str">
+        <f>DistanserMerge!A14</f>
+        <v>Skjennungstua</v>
+      </c>
+      <c r="B14" t="str">
+        <f>DistanserMerge!B14</f>
+        <v>Vensåsseter</v>
+      </c>
+      <c r="C14">
+        <f>DistanserMerge!F14</f>
+        <v>13.5</v>
+      </c>
+      <c r="D14" s="1">
+        <f>DistanserMerge!AG14</f>
+        <v>1.2306293008220623</v>
+      </c>
+      <c r="E14" s="1">
+        <f>DistanserMerge!AJ14</f>
+        <v>1.5756825891472697</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" t="str">
+        <f>DistanserMerge!A15</f>
+        <v>Mellomkollen</v>
+      </c>
+      <c r="B15" t="str">
+        <f>DistanserMerge!B15</f>
+        <v>Fagervann</v>
+      </c>
+      <c r="C15">
+        <f>DistanserMerge!F15</f>
+        <v>5.3</v>
+      </c>
+      <c r="D15" s="1">
+        <f>DistanserMerge!AG15</f>
+        <v>1.5758931221980979</v>
+      </c>
+      <c r="E15" s="1">
+        <f>DistanserMerge!AJ15</f>
+        <v>2.4408199967144131</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" t="str">
+        <f>DistanserMerge!A16</f>
+        <v>Mellomkollen</v>
+      </c>
+      <c r="B16" t="str">
+        <f>DistanserMerge!B16</f>
+        <v>Tømtehyttene</v>
+      </c>
+      <c r="C16">
+        <f>DistanserMerge!F16</f>
+        <v>1.8</v>
+      </c>
+      <c r="D16" s="1">
+        <f>DistanserMerge!AG16</f>
+        <v>1.3085070644454353</v>
+      </c>
+      <c r="E16" s="1">
+        <f>DistanserMerge!AJ16</f>
+        <v>2.5832473443886776</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" t="str">
+        <f>DistanserMerge!A17</f>
+        <v>Mellomkollen</v>
+      </c>
+      <c r="B17" t="str">
+        <f>DistanserMerge!B17</f>
+        <v>Gørja</v>
+      </c>
+      <c r="C17">
+        <f>DistanserMerge!F17</f>
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="D17" s="1">
+        <f>DistanserMerge!AG17</f>
+        <v>1.2738053368753823</v>
+      </c>
+      <c r="E17" s="1">
+        <f>DistanserMerge!AJ17</f>
+        <v>2.396553723974268</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" t="str">
+        <f>DistanserMerge!A18</f>
+        <v>Liggeren</v>
+      </c>
+      <c r="B18" t="str">
+        <f>DistanserMerge!B18</f>
+        <v>Fagervann</v>
+      </c>
+      <c r="C18">
+        <f>DistanserMerge!F18</f>
+        <v>3.8</v>
+      </c>
+      <c r="D18" s="1">
+        <f>DistanserMerge!AG18</f>
+        <v>2.2163208417770912</v>
+      </c>
+      <c r="E18" s="1">
+        <f>DistanserMerge!AJ18</f>
+        <v>1.5236860580980518</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19" t="str">
+        <f>DistanserMerge!A19</f>
+        <v>Liggeren</v>
+      </c>
+      <c r="B19" t="str">
+        <f>DistanserMerge!B19</f>
+        <v>Bjørnholt</v>
+      </c>
+      <c r="C19">
+        <f>DistanserMerge!F19</f>
+        <v>5.4</v>
+      </c>
+      <c r="D19" s="1">
+        <f>DistanserMerge!AG19</f>
+        <v>1.2109943307235786</v>
+      </c>
+      <c r="E19" s="1">
+        <f>DistanserMerge!AJ19</f>
+        <v>1.0334290593311124</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20" t="str">
+        <f>DistanserMerge!A20</f>
+        <v>Liggeren</v>
+      </c>
+      <c r="B20" t="str">
+        <f>DistanserMerge!B20</f>
+        <v>Kikutstua</v>
+      </c>
+      <c r="C20">
+        <f>DistanserMerge!F20</f>
+        <v>6.6</v>
+      </c>
+      <c r="D20" s="1">
+        <f>DistanserMerge!AG20</f>
+        <v>1.671688186030607</v>
+      </c>
+      <c r="E20" s="1">
+        <f>DistanserMerge!AJ20</f>
+        <v>1.5715646186828667</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21" t="str">
+        <f>DistanserMerge!A21</f>
+        <v>Liggeren</v>
+      </c>
+      <c r="B21" t="str">
+        <f>DistanserMerge!B21</f>
+        <v>Gørja</v>
+      </c>
+      <c r="C21">
+        <f>DistanserMerge!F21</f>
+        <v>3.2</v>
+      </c>
+      <c r="D21" s="1">
+        <f>DistanserMerge!AG21</f>
+        <v>2.3812169967190728</v>
+      </c>
+      <c r="E21" s="1">
+        <f>DistanserMerge!AJ21</f>
+        <v>1.9711879143177145</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22" t="str">
+        <f>DistanserMerge!A22</f>
+        <v>Liggeren</v>
+      </c>
+      <c r="B22" t="str">
+        <f>DistanserMerge!B22</f>
+        <v>Tømtehyttene</v>
+      </c>
+      <c r="C22">
+        <f>DistanserMerge!F22</f>
+        <v>1.8</v>
+      </c>
+      <c r="D22" s="1">
+        <f>DistanserMerge!AG22</f>
+        <v>3.6640797982675437</v>
+      </c>
+      <c r="E22" s="1">
+        <f>DistanserMerge!AJ22</f>
+        <v>0.9458379462046782</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23" t="str">
+        <f>DistanserMerge!A23</f>
+        <v>Fagervann (Nord stikryss)</v>
+      </c>
+      <c r="B23" t="str">
+        <f>DistanserMerge!B23</f>
+        <v>Studenterhytta</v>
+      </c>
+      <c r="C23">
+        <f>DistanserMerge!F23</f>
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="D23" s="1">
+        <f>DistanserMerge!AG23</f>
+        <v>1.4602988525407858</v>
+      </c>
+      <c r="E23" s="1">
+        <f>DistanserMerge!AJ23</f>
+        <v>1.6219837260116434</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24" t="str">
+        <f>DistanserMerge!A24</f>
+        <v>Fagervann (Nord stikryss)</v>
+      </c>
+      <c r="B24" t="str">
+        <f>DistanserMerge!B24</f>
+        <v>Bjørnholt</v>
+      </c>
+      <c r="C24">
+        <f>DistanserMerge!F24</f>
+        <v>5.5</v>
+      </c>
+      <c r="D24" s="1">
+        <f>DistanserMerge!AG24</f>
+        <v>1.4969493728367602</v>
+      </c>
+      <c r="E24" s="1">
+        <f>DistanserMerge!AJ24</f>
+        <v>1.8359731448062782</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="A25" t="str">
+        <f>DistanserMerge!A25</f>
+        <v>Fagervann (Nord stikryss)</v>
+      </c>
+      <c r="B25" t="str">
+        <f>DistanserMerge!B25</f>
+        <v>Kobberhaughytta</v>
+      </c>
+      <c r="C25">
+        <f>DistanserMerge!F25</f>
+        <v>8.3000000000000007</v>
+      </c>
+      <c r="D25" s="1">
+        <f>DistanserMerge!AG25</f>
+        <v>1.5843477498268412</v>
+      </c>
+      <c r="E25" s="1">
+        <f>DistanserMerge!AJ25</f>
+        <v>1.6041102345823661</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="A26" t="str">
+        <f>DistanserMerge!A26</f>
+        <v>Fagervann (Nord stikryss)</v>
+      </c>
+      <c r="B26" t="str">
+        <f>DistanserMerge!B26</f>
+        <v>Tømtehyttene</v>
+      </c>
+      <c r="C26">
+        <f>DistanserMerge!F26</f>
+        <v>4.5</v>
+      </c>
+      <c r="D26" s="1">
+        <f>DistanserMerge!AG26</f>
+        <v>2.3563953573504488</v>
+      </c>
+      <c r="E26" s="1">
+        <f>DistanserMerge!AJ26</f>
+        <v>1.9614676272792857</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="A27" t="str">
+        <f>DistanserMerge!A27</f>
+        <v>Studenterhytta</v>
+      </c>
+      <c r="B27" t="str">
+        <f>DistanserMerge!B27</f>
+        <v>Kobberhaughytta</v>
+      </c>
+      <c r="C27">
+        <f>DistanserMerge!F27</f>
+        <v>1.4</v>
+      </c>
+      <c r="D27" s="1">
+        <f>DistanserMerge!AG27</f>
+        <v>1.6931631022718319</v>
+      </c>
+      <c r="E27" s="1">
+        <f>DistanserMerge!AJ27</f>
+        <v>1.0608034478925643</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5">
+      <c r="A28" t="str">
+        <f>DistanserMerge!A28</f>
+        <v>Studenterhytta</v>
+      </c>
+      <c r="B28" t="str">
+        <f>DistanserMerge!B28</f>
+        <v>Brunkollen</v>
+      </c>
+      <c r="C28">
+        <f>DistanserMerge!F28</f>
+        <v>13.9</v>
+      </c>
+      <c r="D28" s="1">
+        <f>DistanserMerge!AG28</f>
+        <v>1.362925872965921</v>
+      </c>
+      <c r="E28" s="1">
+        <f>DistanserMerge!AJ28</f>
+        <v>1.3885495201839113</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5">
+      <c r="A29" t="str">
+        <f>DistanserMerge!A29</f>
+        <v>Studenterhytta</v>
+      </c>
+      <c r="B29" t="str">
+        <f>DistanserMerge!B29</f>
+        <v>Smedmyrkoia</v>
+      </c>
+      <c r="C29">
+        <f>DistanserMerge!F29</f>
+        <v>10.4</v>
+      </c>
+      <c r="D29" s="1">
+        <f>DistanserMerge!AG29</f>
+        <v>1.2522562413356348</v>
+      </c>
+      <c r="E29" s="1">
+        <f>DistanserMerge!AJ29</f>
+        <v>1.4272945078699761</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5">
+      <c r="A30" t="str">
+        <f>DistanserMerge!A30</f>
+        <v>Studenterhytta</v>
+      </c>
+      <c r="B30" t="str">
+        <f>DistanserMerge!B30</f>
+        <v>Vensåsseter</v>
+      </c>
+      <c r="C30">
+        <f>DistanserMerge!F30</f>
+        <v>11.7</v>
+      </c>
+      <c r="D30" s="1">
+        <f>DistanserMerge!AG30</f>
+        <v>1.3823331034734283</v>
+      </c>
+      <c r="E30" s="1">
+        <f>DistanserMerge!AJ30</f>
+        <v>1.5709166786713191</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5">
+      <c r="A31" t="str">
+        <f>DistanserMerge!A31</f>
+        <v>Bjørnholt</v>
+      </c>
+      <c r="B31" t="str">
+        <f>DistanserMerge!B31</f>
+        <v>Kikutstua</v>
+      </c>
+      <c r="C31">
+        <f>DistanserMerge!F31</f>
+        <v>5.35</v>
+      </c>
+      <c r="D31" s="1">
+        <f>DistanserMerge!AG31</f>
+        <v>1.5418145978080204</v>
+      </c>
+      <c r="E31" s="1">
+        <f>DistanserMerge!AJ31</f>
+        <v>1.5687825331972247</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5">
+      <c r="A32" t="str">
+        <f>DistanserMerge!A32</f>
+        <v>Bjørnholt</v>
+      </c>
+      <c r="B32" t="str">
+        <f>DistanserMerge!B32</f>
+        <v>Gørja</v>
+      </c>
+      <c r="C32">
+        <f>DistanserMerge!F32</f>
+        <v>7.2</v>
+      </c>
+      <c r="D32" s="1">
+        <f>DistanserMerge!AG32</f>
+        <v>1.1851301104068048</v>
+      </c>
+      <c r="E32" s="1">
+        <f>DistanserMerge!AJ32</f>
+        <v>1.1385909824018206</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5">
+      <c r="A33" t="str">
+        <f>DistanserMerge!A33</f>
+        <v>Bjørnholt</v>
+      </c>
+      <c r="B33" t="str">
+        <f>DistanserMerge!B33</f>
+        <v>Kobberhaughytta</v>
+      </c>
+      <c r="C33">
+        <f>DistanserMerge!F33</f>
+        <v>2.9</v>
+      </c>
+      <c r="D33" s="1">
+        <f>DistanserMerge!AG33</f>
+        <v>2.7158869255512554</v>
+      </c>
+      <c r="E33" s="1">
+        <f>DistanserMerge!AJ33</f>
+        <v>1.741069157914918</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5">
+      <c r="A34" t="str">
+        <f>DistanserMerge!A34</f>
+        <v>Kikutstua</v>
+      </c>
+      <c r="B34" t="str">
+        <f>DistanserMerge!B34</f>
+        <v>Gørja</v>
+      </c>
+      <c r="C34">
+        <f>DistanserMerge!F34</f>
+        <v>6.8</v>
+      </c>
+      <c r="D34" s="1">
+        <f>DistanserMerge!AG34</f>
+        <v>1.0808362790821178</v>
+      </c>
+      <c r="E34" s="1">
+        <f>DistanserMerge!AJ34</f>
+        <v>0.99262091233455441</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5">
+      <c r="A35" t="str">
+        <f>DistanserMerge!A35</f>
+        <v>Kikutstua</v>
+      </c>
+      <c r="B35" t="str">
+        <f>DistanserMerge!B35</f>
+        <v>Kobberhaughytta</v>
+      </c>
+      <c r="C35">
+        <f>DistanserMerge!F35</f>
+        <v>5.2</v>
+      </c>
+      <c r="D35" s="1">
+        <f>DistanserMerge!AG35</f>
+        <v>1.929907018534871</v>
+      </c>
+      <c r="E35" s="1">
+        <f>DistanserMerge!AJ35</f>
+        <v>1.444840671631441</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5">
+      <c r="A36" t="str">
+        <f>DistanserMerge!A36</f>
+        <v>Kikutstua</v>
+      </c>
+      <c r="B36" t="str">
+        <f>DistanserMerge!B36</f>
+        <v>Smedmyrkoia</v>
+      </c>
+      <c r="C36">
+        <f>DistanserMerge!F36</f>
+        <v>13.6</v>
+      </c>
+      <c r="D36" s="1">
+        <f>DistanserMerge!AG36</f>
+        <v>1.3892298781072241</v>
+      </c>
+      <c r="E36" s="1">
+        <f>DistanserMerge!AJ36</f>
+        <v>1.4074244220449721</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5">
+      <c r="A37" t="str">
+        <f>DistanserMerge!A37</f>
+        <v>Kikutstua</v>
+      </c>
+      <c r="B37" t="str">
+        <f>DistanserMerge!B37</f>
+        <v>Oppkuven</v>
+      </c>
+      <c r="C37">
+        <f>DistanserMerge!F37</f>
+        <v>11.9</v>
+      </c>
+      <c r="D37" s="1">
+        <f>DistanserMerge!AG37</f>
+        <v>2.121258273793476</v>
+      </c>
+      <c r="E37" s="1">
+        <f>DistanserMerge!AJ37</f>
+        <v>1.236327326006583</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5">
+      <c r="A39" t="str">
+        <f>DistanserMerge!A39</f>
+        <v>Gørja (hytta)</v>
+      </c>
+      <c r="B39" t="str">
+        <f>DistanserMerge!B39</f>
+        <v>Tømtehyttene</v>
+      </c>
+      <c r="C39">
+        <f>DistanserMerge!F39</f>
+        <v>4</v>
+      </c>
+      <c r="D39" s="1">
+        <f>DistanserMerge!AG39</f>
+        <v>2.191203731100372</v>
+      </c>
+      <c r="E39" s="1">
+        <f>DistanserMerge!AJ39</f>
+        <v>1.3983033720889129</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5">
+      <c r="A40" t="str">
+        <f>DistanserMerge!A40</f>
+        <v>Kobberhaughytta</v>
+      </c>
+      <c r="B40" t="str">
+        <f>DistanserMerge!B40</f>
+        <v>Smedmyrkoia</v>
+      </c>
+      <c r="C40">
+        <f>DistanserMerge!F40</f>
+        <v>11.1</v>
+      </c>
+      <c r="D40" s="1">
+        <f>DistanserMerge!AG40</f>
+        <v>1.2612387083021073</v>
+      </c>
+      <c r="E40" s="1">
+        <f>DistanserMerge!AJ40</f>
+        <v>1.5328555974387879</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5">
+      <c r="A41" t="str">
+        <f>DistanserMerge!A41</f>
+        <v>Brunkollen</v>
+      </c>
+      <c r="B41" t="str">
+        <f>DistanserMerge!B41</f>
+        <v>Sæteren</v>
+      </c>
+      <c r="C41">
+        <f>DistanserMerge!F41</f>
+        <v>3.4</v>
+      </c>
+      <c r="D41" s="1">
+        <f>DistanserMerge!AG41</f>
+        <v>0.99328238236521438</v>
+      </c>
+      <c r="E41" s="1">
+        <f>DistanserMerge!AJ41</f>
+        <v>3.2442366058530192</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5">
+      <c r="A42" t="str">
+        <f>DistanserMerge!A42</f>
+        <v>Brunkollen</v>
+      </c>
+      <c r="B42" t="str">
+        <f>DistanserMerge!B42</f>
+        <v>Vensåsseter</v>
+      </c>
+      <c r="C42">
+        <f>DistanserMerge!F42</f>
+        <v>5.3</v>
+      </c>
+      <c r="D42" s="1">
+        <f>DistanserMerge!AG42</f>
+        <v>1.6259295920135726</v>
+      </c>
+      <c r="E42" s="1">
+        <f>DistanserMerge!AJ42</f>
+        <v>1.9656639239763547</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5">
+      <c r="A43" t="str">
+        <f>DistanserMerge!A43</f>
+        <v>Brunkollen</v>
+      </c>
+      <c r="B43" t="str">
+        <f>DistanserMerge!B43</f>
+        <v>Mustadkroken</v>
+      </c>
+      <c r="C43">
+        <f>DistanserMerge!F43</f>
+        <v>15.4</v>
+      </c>
+      <c r="D43" s="1">
+        <f>DistanserMerge!AG43</f>
+        <v>1.5107757905075316</v>
+      </c>
+      <c r="E43" s="1">
+        <f>DistanserMerge!AJ43</f>
+        <v>1.5508233696359475</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5">
+      <c r="A44" t="str">
+        <f>DistanserMerge!A44</f>
+        <v>Smedmyrkoia</v>
+      </c>
+      <c r="B44" t="str">
+        <f>DistanserMerge!B44</f>
+        <v>Vensåsseter</v>
+      </c>
+      <c r="C44">
+        <f>DistanserMerge!F44</f>
+        <v>9.4</v>
+      </c>
+      <c r="D44" s="1">
+        <f>DistanserMerge!AG44</f>
+        <v>1.6078369999628332</v>
+      </c>
+      <c r="E44" s="1">
+        <f>DistanserMerge!AJ44</f>
+        <v>1.6503941818883239</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5">
+      <c r="A45" t="str">
+        <f>DistanserMerge!A45</f>
+        <v>Smedmyrkoia</v>
+      </c>
+      <c r="B45" t="str">
+        <f>DistanserMerge!B45</f>
+        <v>Myrseter</v>
+      </c>
+      <c r="C45">
+        <f>DistanserMerge!F45</f>
+        <v>13.9</v>
+      </c>
+      <c r="D45" s="1">
+        <f>DistanserMerge!AG45</f>
+        <v>1.5413885560229956</v>
+      </c>
+      <c r="E45" s="1">
+        <f>DistanserMerge!AJ45</f>
+        <v>1.5734860485207223</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5">
+      <c r="A46" t="str">
+        <f>DistanserMerge!A46</f>
+        <v>Smedmyrkoia</v>
+      </c>
+      <c r="B46" t="str">
+        <f>DistanserMerge!B46</f>
+        <v>Oppkuven</v>
+      </c>
+      <c r="C46">
+        <f>DistanserMerge!F46</f>
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="D46" s="1">
+        <f>DistanserMerge!AG46</f>
+        <v>3.3286610060857158</v>
+      </c>
+      <c r="E46" s="1">
+        <f>DistanserMerge!AJ46</f>
+        <v>0.93275803713606453</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5">
+      <c r="A47" t="str">
+        <f>DistanserMerge!A47</f>
+        <v>Smedmyrkoia</v>
+      </c>
+      <c r="B47" t="str">
+        <f>DistanserMerge!B47</f>
+        <v>Presthytta</v>
+      </c>
+      <c r="C47">
+        <f>DistanserMerge!F47</f>
+        <v>12.8</v>
+      </c>
+      <c r="D47" s="1">
+        <f>DistanserMerge!AG47</f>
+        <v>1.8396743604909522</v>
+      </c>
+      <c r="E47" s="1">
+        <f>DistanserMerge!AJ47</f>
+        <v>1.5214289200703974</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5">
+      <c r="A49" t="str">
+        <f>DistanserMerge!A49</f>
+        <v>Vensåsseter</v>
+      </c>
+      <c r="B49" t="str">
+        <f>DistanserMerge!B49</f>
+        <v>Mustadkroken</v>
+      </c>
+      <c r="C49">
+        <f>DistanserMerge!F49</f>
+        <v>14.7</v>
+      </c>
+      <c r="D49" s="1">
+        <f>DistanserMerge!AG49</f>
+        <v>1.7231044763899588</v>
+      </c>
+      <c r="E49" s="1">
+        <f>DistanserMerge!AJ49</f>
+        <v>1.6975998031702271</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5">
+      <c r="A50" t="str">
+        <f>DistanserMerge!A50</f>
+        <v>Vensåsseter</v>
+      </c>
+      <c r="B50" t="str">
+        <f>DistanserMerge!B50</f>
+        <v>Myrseter</v>
+      </c>
+      <c r="C50">
+        <f>DistanserMerge!F50</f>
+        <v>9.8000000000000007</v>
+      </c>
+      <c r="D50" s="1">
+        <f>DistanserMerge!AG50</f>
+        <v>1.5653980236259017</v>
+      </c>
+      <c r="E50" s="1">
+        <f>DistanserMerge!AJ50</f>
+        <v>1.5619548374326193</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5">
+      <c r="A51" t="str">
+        <f>DistanserMerge!A51</f>
+        <v>Vensåsseter</v>
+      </c>
+      <c r="B51" t="str">
+        <f>DistanserMerge!B51</f>
+        <v>Presthytta</v>
+      </c>
+      <c r="C51">
+        <f>DistanserMerge!F51</f>
+        <v>9.1999999999999993</v>
+      </c>
+      <c r="D51" s="1">
+        <f>DistanserMerge!AG51</f>
+        <v>2.0193454515471485</v>
+      </c>
+      <c r="E51" s="1">
+        <f>DistanserMerge!AJ51</f>
+        <v>1.4897595811345758</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5">
+      <c r="A52" t="str">
+        <f>DistanserMerge!A52</f>
+        <v>Mustadkroken</v>
+      </c>
+      <c r="B52" t="str">
+        <f>DistanserMerge!B52</f>
+        <v>Myrseter</v>
+      </c>
+      <c r="C52">
+        <f>DistanserMerge!F52</f>
+        <v>12.8</v>
+      </c>
+      <c r="D52" s="1">
+        <f>DistanserMerge!AG52</f>
+        <v>1.7033456451063449</v>
+      </c>
+      <c r="E52" s="1">
+        <f>DistanserMerge!AJ52</f>
+        <v>1.9098375017486577</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5">
+      <c r="A53" t="str">
+        <f>DistanserMerge!A53</f>
+        <v>Mustadkroken</v>
+      </c>
+      <c r="B53" t="str">
+        <f>DistanserMerge!B53</f>
+        <v>Jørgenhytta</v>
+      </c>
+      <c r="C53">
+        <f>DistanserMerge!F53</f>
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="D53" s="1">
+        <f>DistanserMerge!AG53</f>
+        <v>1.2650153060492619</v>
+      </c>
+      <c r="E53" s="1">
+        <f>DistanserMerge!AJ53</f>
+        <v>1.0671170244893728</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5">
+      <c r="A54" t="str">
+        <f>DistanserMerge!A54</f>
+        <v>Myrseter</v>
+      </c>
+      <c r="B54" t="str">
+        <f>DistanserMerge!B54</f>
+        <v>Presthytta</v>
+      </c>
+      <c r="C54">
+        <f>DistanserMerge!F54</f>
+        <v>3</v>
+      </c>
+      <c r="D54" s="1">
+        <f>DistanserMerge!AG54</f>
+        <v>1.8576246138128709</v>
+      </c>
+      <c r="E54" s="1">
+        <f>DistanserMerge!AJ54</f>
+        <v>0.84222545734048648</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5">
+      <c r="A55" t="str">
+        <f>DistanserMerge!A55</f>
+        <v>Myrseter</v>
+      </c>
+      <c r="B55" t="str">
+        <f>DistanserMerge!B55</f>
+        <v>Jørgenhytta</v>
+      </c>
+      <c r="C55">
+        <f>DistanserMerge!F55</f>
+        <v>7.9</v>
+      </c>
+      <c r="D55" s="1">
+        <f>DistanserMerge!AG55</f>
+        <v>2.0931163880910382</v>
+      </c>
+      <c r="E55" s="1">
+        <f>DistanserMerge!AJ55</f>
+        <v>1.5205196113619515</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5">
+      <c r="A56" t="str">
+        <f>DistanserMerge!A56</f>
+        <v>Oppkuven</v>
+      </c>
+      <c r="B56" t="str">
+        <f>DistanserMerge!B56</f>
+        <v>Presthytta</v>
+      </c>
+      <c r="C56">
+        <f>DistanserMerge!F56</f>
+        <v>11.6</v>
+      </c>
+      <c r="D56" s="1">
+        <f>DistanserMerge!AG56</f>
+        <v>1.336190791495061</v>
+      </c>
+      <c r="E56" s="1">
+        <f>DistanserMerge!AJ56</f>
+        <v>2.1245023339192413</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5">
+      <c r="A57" t="str">
+        <f>DistanserMerge!A57</f>
+        <v>Oppkuven</v>
+      </c>
+      <c r="B57" t="str">
+        <f>DistanserMerge!B57</f>
+        <v>Gyrihaugen</v>
+      </c>
+      <c r="C57">
+        <f>DistanserMerge!F57</f>
+        <v>11.350000000000001</v>
+      </c>
+      <c r="D57" s="1">
+        <f>DistanserMerge!AG57</f>
+        <v>1.6894536332068473</v>
+      </c>
+      <c r="E57" s="1">
+        <f>DistanserMerge!AJ57</f>
+        <v>1.7856199507658617</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5">
+      <c r="A58" t="str">
+        <f>DistanserMerge!A58</f>
+        <v>Oppkuven</v>
+      </c>
+      <c r="B58" t="str">
+        <f>DistanserMerge!B58</f>
+        <v>Sinnerdammen</v>
+      </c>
+      <c r="C58">
+        <f>DistanserMerge!F58</f>
+        <v>14.4</v>
+      </c>
+      <c r="D58" s="1">
+        <f>DistanserMerge!AG58</f>
+        <v>1.1255563327306679</v>
+      </c>
+      <c r="E58" s="1">
+        <f>DistanserMerge!AJ58</f>
+        <v>1.5441079588825262</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5">
+      <c r="A59" t="str">
+        <f>DistanserMerge!A59</f>
+        <v>Oppkuven</v>
+      </c>
+      <c r="B59" t="str">
+        <f>DistanserMerge!B59</f>
+        <v>Katnosdammen</v>
+      </c>
+      <c r="C59">
+        <f>DistanserMerge!F59</f>
+        <v>14.1</v>
+      </c>
+      <c r="D59" s="1">
+        <f>DistanserMerge!AG59</f>
+        <v>1.3055305229229142</v>
+      </c>
+      <c r="E59" s="1">
+        <f>DistanserMerge!AJ59</f>
+        <v>1.8410592626584539</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5">
+      <c r="A60" t="str">
+        <f>DistanserMerge!A60</f>
+        <v>Presthytta</v>
+      </c>
+      <c r="B60" t="str">
+        <f>DistanserMerge!B60</f>
+        <v>Gyrihaugen</v>
+      </c>
+      <c r="C60">
+        <f>DistanserMerge!F60</f>
+        <v>6.5</v>
+      </c>
+      <c r="D60" s="1">
+        <f>DistanserMerge!AG60</f>
+        <v>2.0916704677566318</v>
+      </c>
+      <c r="E60" s="1">
+        <f>DistanserMerge!AJ60</f>
+        <v>0.94288112900170928</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5">
+      <c r="A61" t="str">
+        <f>DistanserMerge!A61</f>
+        <v>Gyrihaugen</v>
+      </c>
+      <c r="B61" t="str">
+        <f>DistanserMerge!B61</f>
+        <v>Sinnerdammen</v>
+      </c>
+      <c r="C61">
+        <f>DistanserMerge!F61</f>
+        <v>15</v>
+      </c>
+      <c r="D61" s="1">
+        <f>DistanserMerge!AG61</f>
+        <v>1.3333168510319342</v>
+      </c>
+      <c r="E61" s="1">
+        <f>DistanserMerge!AJ61</f>
+        <v>1.6619592659196001</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5">
+      <c r="A62" t="str">
+        <f>DistanserMerge!A62</f>
+        <v>Sinnerdammen</v>
+      </c>
+      <c r="B62" t="str">
+        <f>DistanserMerge!B62</f>
+        <v>Pershusfjellet</v>
+      </c>
+      <c r="C62">
+        <f>DistanserMerge!F62</f>
+        <v>3.4</v>
+      </c>
+      <c r="D62" s="1">
+        <f>DistanserMerge!AG62</f>
+        <v>2.0477328945116144</v>
+      </c>
+      <c r="E62" s="1">
+        <f>DistanserMerge!AJ62</f>
+        <v>1.2908890847215617</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5">
+      <c r="A63" t="str">
+        <f>DistanserMerge!A63</f>
+        <v>Sinnerdammen</v>
+      </c>
+      <c r="B63" t="str">
+        <f>DistanserMerge!B63</f>
+        <v>Katnosdammen</v>
+      </c>
+      <c r="C63">
+        <f>DistanserMerge!F63</f>
+        <v>7.5</v>
+      </c>
+      <c r="D63" s="1">
+        <f>DistanserMerge!AG63</f>
+        <v>1.6472168441799986</v>
+      </c>
+      <c r="E63" s="1">
+        <f>DistanserMerge!AJ63</f>
+        <v>1.7100384336498959</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5">
+      <c r="A64" t="str">
+        <f>DistanserMerge!A64</f>
+        <v>Pershusfjellet</v>
+      </c>
+      <c r="B64" t="str">
+        <f>DistanserMerge!B64</f>
+        <v>Katnosdammen</v>
+      </c>
+      <c r="C64">
+        <f>DistanserMerge!F64</f>
+        <v>10.199999999999999</v>
+      </c>
+      <c r="D64" s="1">
+        <f>DistanserMerge!AG64</f>
+        <v>1.5937521055725425</v>
+      </c>
+      <c r="E64" s="1">
+        <f>DistanserMerge!AJ64</f>
+        <v>1.949077837868342</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.78740157499999996" right="0.78740157499999996" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>